<commit_message>
add links to EQUATES activity data
</commit_message>
<xml_diff>
--- a/_transportation/data-raw/epa/epa_downloads.xlsx
+++ b/_transportation/data-raw/epa/epa_downloads.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotenle/Documents/MetC_Locals/Interdivisional/ghg-cprg/_transportation/data-raw/epa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FA0167-2457-5A42-9D02-C6A223CD691F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C94C37-8069-664B-98F1-295F6EB6DB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="500" windowWidth="30720" windowHeight="17040" xr2:uid="{E3501ACA-8D46-AF4B-AC5D-95BB483C9130}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17040" xr2:uid="{E3501ACA-8D46-AF4B-AC5D-95BB483C9130}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="205">
   <si>
     <t>file_name</t>
   </si>
@@ -635,6 +635,27 @@
   </si>
   <si>
     <t>2018v2/2018gc_cb6_18j</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/Air/emismod/MOVES3/other_inputs/2002repCDBs_20201028.zip</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/Air/emismod/MOVES3/other_inputs/2005repCDBs_20201028.zip</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/Air/emismod/MOVES3/other_inputs/2008repCDBs_20201016.zip</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/Air/emismod/MOVES3/other_inputs/2011repCDBs_20201016.zip</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/Air/emismod/MOVES3/other_inputs/2014repCDBs_20201027.zip</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/Air/emismod/MOVES3/2017/2017repCDBs_20201209.zip</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/Air/emismod/MOVES3/2017/EQUATES_2017_inventory_onroad_activity_11jan2021.zip</t>
   </si>
 </sst>
 </file>
@@ -711,15 +732,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -731,6 +749,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1183,10 +1205,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8EF959-18DF-BD43-B878-2D065289D72D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H137"/>
+  <dimension ref="A1:H144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="123" workbookViewId="0">
-      <selection activeCell="A125" sqref="A125"/>
+    <sheetView tabSelected="1" topLeftCell="F79" zoomScale="123" workbookViewId="0">
+      <selection activeCell="A109" sqref="A1:H144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1197,11 +1219,11 @@
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="62.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="62.6640625" style="12" customWidth="1"/>
     <col min="8" max="8" width="115.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1220,34 +1242,34 @@
       <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="5" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="7">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6">
         <v>2001</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="9" t="s">
+      <c r="D2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:8" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1265,50 +1287,49 @@
         <v>68</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="7">
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6">
         <v>2001</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="9" t="s">
+      <c r="D4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="5" t="s">
-        <v>69</v>
-      </c>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5"/>
     </row>
     <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1323,6 +1344,7 @@
       <c r="D6" t="s">
         <v>150</v>
       </c>
+      <c r="G6" s="1"/>
       <c r="H6" t="s">
         <v>160</v>
       </c>
@@ -1360,16 +1382,17 @@
       <c r="F8" t="s">
         <v>66</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="G8" s="1"/>
+      <c r="H8" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>2002</v>
+        <v>2005</v>
       </c>
       <c r="C9" t="s">
         <v>50</v>
@@ -1377,7 +1400,7 @@
       <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="12" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1386,79 +1409,71 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>2002</v>
+        <v>2008</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
-      <c r="F10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="G10" s="12" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>2002</v>
+        <v>2011</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="H11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12">
-        <v>2003</v>
+        <v>2012</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13">
-        <v>2004</v>
+        <v>2013</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1473,6 +1488,7 @@
       <c r="D14" t="s">
         <v>150</v>
       </c>
+      <c r="G14" s="1"/>
       <c r="H14" t="s">
         <v>161</v>
       </c>
@@ -1578,16 +1594,17 @@
       <c r="F20" t="s">
         <v>64</v>
       </c>
+      <c r="G20" s="1"/>
       <c r="H20" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
       <c r="B21">
-        <v>2005</v>
+        <v>2014</v>
       </c>
       <c r="C21" t="s">
         <v>50</v>
@@ -1595,77 +1612,74 @@
       <c r="D21" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B22">
-        <v>2005</v>
+        <v>2015</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D22" t="s">
         <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="H22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>7</v>
       </c>
       <c r="B23">
-        <v>2005</v>
+        <v>2015</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>194</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="H23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>7</v>
       </c>
       <c r="B24">
-        <v>2005</v>
+        <v>2016</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D24" t="s">
         <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>194</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="H24" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
@@ -1684,6 +1698,7 @@
       <c r="F25" t="s">
         <v>163</v>
       </c>
+      <c r="G25" s="1"/>
       <c r="H25" t="s">
         <v>162</v>
       </c>
@@ -1722,61 +1737,64 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>7</v>
       </c>
       <c r="B28">
-        <v>2006</v>
+        <v>2017</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>7</v>
       </c>
       <c r="B29">
-        <v>2007</v>
+        <v>2018</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>196</v>
+      </c>
+      <c r="H29" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="B30">
-        <v>2008</v>
+        <v>2019</v>
       </c>
       <c r="C30" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>127</v>
+        <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>131</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="H30" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -1846,6 +1864,7 @@
       <c r="F34" t="s">
         <v>61</v>
       </c>
+      <c r="G34" s="1"/>
       <c r="H34" t="s">
         <v>62</v>
       </c>
@@ -1866,62 +1885,57 @@
       <c r="F35" t="s">
         <v>93</v>
       </c>
+      <c r="G35" s="1"/>
       <c r="H35" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="B36">
-        <v>2008</v>
+        <v>2020</v>
       </c>
       <c r="C36" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="D36" t="s">
-        <v>127</v>
+        <v>10</v>
       </c>
       <c r="F36" t="s">
-        <v>131</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+      <c r="H36" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="B37">
-        <v>2008</v>
+        <v>2021</v>
       </c>
       <c r="C37" t="s">
-        <v>126</v>
+        <v>50</v>
       </c>
       <c r="D37" t="s">
-        <v>127</v>
+        <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>131</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+      <c r="H37" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>7</v>
       </c>
       <c r="B38">
-        <v>2008</v>
+        <v>2022</v>
       </c>
       <c r="C38" t="s">
         <v>50</v>
@@ -1929,16 +1943,19 @@
       <c r="D38" t="s">
         <v>10</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>193</v>
+      <c r="F38" t="s">
+        <v>83</v>
+      </c>
+      <c r="H38" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="B39">
-        <v>2008</v>
+        <v>2001</v>
       </c>
       <c r="C39" t="s">
         <v>48</v>
@@ -1946,11 +1963,13 @@
       <c r="D39" t="s">
         <v>10</v>
       </c>
-      <c r="F39" t="s">
-        <v>61</v>
-      </c>
-      <c r="H39" t="s">
-        <v>92</v>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="G39" s="13"/>
+      <c r="H39" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1958,7 +1977,7 @@
         <v>7</v>
       </c>
       <c r="B40">
-        <v>2008</v>
+        <v>2002</v>
       </c>
       <c r="C40" t="s">
         <v>48</v>
@@ -1967,18 +1986,18 @@
         <v>10</v>
       </c>
       <c r="F40" t="s">
-        <v>61</v>
-      </c>
-      <c r="H40" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B41">
-        <v>2008</v>
+        <v>2003</v>
       </c>
       <c r="C41" t="s">
         <v>48</v>
@@ -1986,15 +2005,10 @@
       <c r="D41" t="s">
         <v>10</v>
       </c>
-      <c r="F41" t="s">
-        <v>24</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H41" t="s">
-        <v>32</v>
-      </c>
+      <c r="G41" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="H41" s="3"/>
     </row>
     <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -2009,6 +2023,7 @@
       <c r="D42" t="s">
         <v>150</v>
       </c>
+      <c r="G42" s="1"/>
       <c r="H42" t="s">
         <v>164</v>
       </c>
@@ -2029,6 +2044,7 @@
       <c r="F43" t="s">
         <v>179</v>
       </c>
+      <c r="G43" s="1"/>
       <c r="H43" t="s">
         <v>172</v>
       </c>
@@ -2120,7 +2136,7 @@
       <c r="G48" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H48" s="4" t="s">
+      <c r="H48" s="3" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2143,7 +2159,7 @@
       <c r="G49" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H49" s="4" t="s">
+      <c r="H49" s="3" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2163,6 +2179,7 @@
       <c r="F50" t="s">
         <v>120</v>
       </c>
+      <c r="G50" s="1"/>
       <c r="H50" t="s">
         <v>125</v>
       </c>
@@ -2183,16 +2200,17 @@
       <c r="F51" t="s">
         <v>90</v>
       </c>
+      <c r="G51" s="1"/>
       <c r="H51" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>7</v>
       </c>
       <c r="B52">
-        <v>2009</v>
+        <v>2004</v>
       </c>
       <c r="C52" t="s">
         <v>48</v>
@@ -2200,16 +2218,17 @@
       <c r="D52" t="s">
         <v>10</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="G52" s="12" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="H52" s="3"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>7</v>
       </c>
       <c r="B53">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="C53" t="s">
         <v>48</v>
@@ -2217,54 +2236,54 @@
       <c r="D53" t="s">
         <v>10</v>
       </c>
-      <c r="G53" s="1" t="s">
+      <c r="F53" t="s">
+        <v>194</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54">
+        <v>2005</v>
+      </c>
+      <c r="C54" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" t="s">
+        <v>194</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H54" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55">
+        <v>2006</v>
+      </c>
+      <c r="C55" t="s">
+        <v>48</v>
+      </c>
+      <c r="D55" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" s="12" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>73</v>
-      </c>
-      <c r="B54">
-        <v>2011</v>
-      </c>
-      <c r="C54" t="s">
-        <v>115</v>
-      </c>
-      <c r="D54" t="s">
-        <v>10</v>
-      </c>
-      <c r="F54" t="s">
-        <v>120</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H54" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>73</v>
-      </c>
-      <c r="B55">
-        <v>2011</v>
-      </c>
-      <c r="C55" t="s">
-        <v>115</v>
-      </c>
-      <c r="D55" t="s">
-        <v>10</v>
-      </c>
-      <c r="F55" t="s">
-        <v>120</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H55" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -2272,27 +2291,24 @@
         <v>7</v>
       </c>
       <c r="B56">
-        <v>2011</v>
+        <v>2007</v>
       </c>
       <c r="C56" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D56" t="s">
         <v>10</v>
       </c>
-      <c r="F56" t="s">
-        <v>53</v>
-      </c>
-      <c r="H56" t="s">
-        <v>54</v>
+      <c r="G56" s="12" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="B57">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="C57" t="s">
         <v>48</v>
@@ -2301,18 +2317,18 @@
         <v>10</v>
       </c>
       <c r="F57" t="s">
-        <v>120</v>
+        <v>61</v>
       </c>
       <c r="H57" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>7</v>
       </c>
       <c r="B58">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="C58" t="s">
         <v>48</v>
@@ -2320,22 +2336,16 @@
       <c r="D58" t="s">
         <v>10</v>
       </c>
-      <c r="F58" t="s">
-        <v>59</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H58" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="G58" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>7</v>
       </c>
       <c r="B59">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="C59" t="s">
         <v>48</v>
@@ -2343,19 +2353,13 @@
       <c r="D59" t="s">
         <v>10</v>
       </c>
-      <c r="F59" t="s">
-        <v>59</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H59" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="G59" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B60">
         <v>2011</v>
@@ -2367,13 +2371,13 @@
         <v>10</v>
       </c>
       <c r="F60" t="s">
-        <v>25</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
+      </c>
+      <c r="G60" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="H60" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
@@ -2392,6 +2396,7 @@
       <c r="F61" t="s">
         <v>166</v>
       </c>
+      <c r="G61" s="1"/>
       <c r="H61" t="s">
         <v>165</v>
       </c>
@@ -2412,6 +2417,7 @@
       <c r="F62" t="s">
         <v>177</v>
       </c>
+      <c r="G62" s="1"/>
       <c r="H62" t="s">
         <v>175</v>
       </c>
@@ -2468,24 +2474,24 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B66" s="5">
+      <c r="A66" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" s="4">
         <v>2013</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D66" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="6" t="s">
+      <c r="D66" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H66" s="5"/>
+      <c r="H66" s="4"/>
     </row>
     <row r="67" spans="1:8" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
@@ -2504,24 +2510,30 @@
         <v>98</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>7</v>
       </c>
       <c r="B68">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="C68" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D68" t="s">
         <v>10</v>
       </c>
-      <c r="G68" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="F68" t="s">
+        <v>59</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H68" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -2534,11 +2546,11 @@
       <c r="D69" t="s">
         <v>10</v>
       </c>
-      <c r="G69" s="1" t="s">
+      <c r="G69" s="12" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -2546,21 +2558,21 @@
         <v>2013</v>
       </c>
       <c r="C70" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D70" t="s">
         <v>10</v>
       </c>
-      <c r="G70" s="1" t="s">
+      <c r="G70" s="12" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>7</v>
       </c>
       <c r="B71">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="C71" t="s">
         <v>48</v>
@@ -2568,8 +2580,11 @@
       <c r="D71" t="s">
         <v>10</v>
       </c>
-      <c r="G71" s="1" t="s">
-        <v>98</v>
+      <c r="F71" t="s">
+        <v>41</v>
+      </c>
+      <c r="H71" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -2605,6 +2620,7 @@
       <c r="F73" t="s">
         <v>109</v>
       </c>
+      <c r="G73" s="1"/>
       <c r="H73" t="s">
         <v>108</v>
       </c>
@@ -2625,27 +2641,29 @@
       <c r="F74" t="s">
         <v>107</v>
       </c>
+      <c r="G74" s="1"/>
       <c r="H74" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B75" s="5">
+      <c r="A75" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B75" s="4">
         <v>2014</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C75" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D75" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F75" s="5" t="s">
+      <c r="D75" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F75" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="H75" s="4" t="s">
+      <c r="G75" s="1"/>
+      <c r="H75" s="3" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2662,10 +2680,11 @@
       <c r="D76" t="s">
         <v>16</v>
       </c>
-      <c r="F76" s="5" t="s">
+      <c r="F76" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="H76" s="4" t="s">
+      <c r="G76" s="1"/>
+      <c r="H76" s="3" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2685,6 +2704,7 @@
       <c r="F77" t="s">
         <v>87</v>
       </c>
+      <c r="G77" s="1"/>
       <c r="H77" t="s">
         <v>88</v>
       </c>
@@ -2694,47 +2714,47 @@
         <v>7</v>
       </c>
       <c r="B78">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="C78" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D78" t="s">
         <v>10</v>
       </c>
       <c r="F78" t="s">
-        <v>95</v>
+        <v>38</v>
       </c>
       <c r="H78" t="s">
-        <v>96</v>
+        <v>39</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="B79">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="C79" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D79" t="s">
         <v>10</v>
       </c>
       <c r="F79" t="s">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="H79" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="B80">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="C80" t="s">
         <v>48</v>
@@ -2743,10 +2763,10 @@
         <v>10</v>
       </c>
       <c r="F80" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="H80" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -2754,7 +2774,7 @@
         <v>7</v>
       </c>
       <c r="B81">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="C81" t="s">
         <v>48</v>
@@ -2763,18 +2783,18 @@
         <v>10</v>
       </c>
       <c r="F81" t="s">
-        <v>41</v>
+        <v>197</v>
       </c>
       <c r="H81" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B82">
-        <v>2014</v>
+        <v>2019</v>
       </c>
       <c r="C82" t="s">
         <v>48</v>
@@ -2783,13 +2803,10 @@
         <v>10</v>
       </c>
       <c r="F82" t="s">
-        <v>26</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="H82" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="17" hidden="1" x14ac:dyDescent="0.2">
@@ -2825,6 +2842,7 @@
       <c r="F84" t="s">
         <v>178</v>
       </c>
+      <c r="G84" s="1"/>
       <c r="H84" t="s">
         <v>176</v>
       </c>
@@ -2845,6 +2863,7 @@
       <c r="F85" t="s">
         <v>38</v>
       </c>
+      <c r="G85" s="1"/>
       <c r="H85" t="s">
         <v>49</v>
       </c>
@@ -2865,69 +2884,70 @@
       <c r="G86" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="H86" s="4"/>
+      <c r="H86" s="3"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>7</v>
       </c>
       <c r="B87">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="C87" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D87" t="s">
         <v>10</v>
       </c>
       <c r="F87" t="s">
-        <v>38</v>
-      </c>
-      <c r="H87" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>7</v>
-      </c>
-      <c r="B88">
-        <v>2015</v>
-      </c>
-      <c r="C88" t="s">
-        <v>50</v>
-      </c>
-      <c r="D88" t="s">
-        <v>10</v>
-      </c>
-      <c r="F88" t="s">
-        <v>38</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="H88" t="s">
-        <v>167</v>
+        <v>37</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B88" s="4">
+        <v>2021</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E88" s="4"/>
+      <c r="F88" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G88" s="13"/>
+      <c r="H88" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>7</v>
-      </c>
-      <c r="B89">
-        <v>2015</v>
-      </c>
-      <c r="C89" t="s">
-        <v>48</v>
-      </c>
-      <c r="D89" t="s">
-        <v>10</v>
-      </c>
-      <c r="F89" t="s">
-        <v>38</v>
-      </c>
-      <c r="H89" t="s">
-        <v>39</v>
+      <c r="A89" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B89" s="4">
+        <v>2022</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G89" s="13"/>
+      <c r="H89" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
@@ -2943,6 +2963,7 @@
       <c r="D90" t="s">
         <v>150</v>
       </c>
+      <c r="G90" s="1"/>
       <c r="H90" t="s">
         <v>168</v>
       </c>
@@ -2963,6 +2984,7 @@
       <c r="F91" t="s">
         <v>145</v>
       </c>
+      <c r="G91" s="1"/>
       <c r="H91" t="s">
         <v>144</v>
       </c>
@@ -2983,48 +3005,43 @@
       <c r="F92" t="s">
         <v>105</v>
       </c>
+      <c r="G92" s="1"/>
       <c r="H92" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>7</v>
-      </c>
-      <c r="B93">
-        <v>2016</v>
-      </c>
-      <c r="C93" t="s">
-        <v>50</v>
-      </c>
-      <c r="D93" t="s">
-        <v>10</v>
-      </c>
-      <c r="F93" t="s">
-        <v>105</v>
+      <c r="A93" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" s="4">
+        <v>2002</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="H93" t="s">
-        <v>104</v>
+        <v>198</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>7</v>
-      </c>
-      <c r="B94">
-        <v>2016</v>
-      </c>
-      <c r="C94" t="s">
-        <v>48</v>
-      </c>
-      <c r="D94" t="s">
-        <v>10</v>
-      </c>
-      <c r="F94" t="s">
-        <v>44</v>
+      <c r="A94" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" s="4">
+        <v>2005</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="H94" t="s">
-        <v>15</v>
+        <v>199</v>
       </c>
     </row>
     <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
@@ -3040,6 +3057,7 @@
       <c r="D95" t="s">
         <v>150</v>
       </c>
+      <c r="G95" s="1"/>
       <c r="H95" t="s">
         <v>169</v>
       </c>
@@ -3060,6 +3078,7 @@
       <c r="F96" t="s">
         <v>114</v>
       </c>
+      <c r="G96" s="1"/>
       <c r="H96" t="s">
         <v>113</v>
       </c>
@@ -3097,6 +3116,7 @@
       <c r="F98" t="s">
         <v>45</v>
       </c>
+      <c r="G98" s="1"/>
       <c r="H98" t="s">
         <v>47</v>
       </c>
@@ -3117,111 +3137,94 @@
       <c r="F99" t="s">
         <v>77</v>
       </c>
+      <c r="G99" s="1"/>
       <c r="H99" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>7</v>
-      </c>
-      <c r="B100">
+      <c r="A100" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B100" s="4">
+        <v>2008</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H100" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B101" s="4">
+        <v>2011</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H101" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B102" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H102" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B103" s="4">
         <v>2017</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C103" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H103" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B104" s="4">
+        <v>2017</v>
+      </c>
+      <c r="C104" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D100" t="s">
-        <v>10</v>
-      </c>
-      <c r="F100" t="s">
-        <v>14</v>
-      </c>
-      <c r="H100" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>73</v>
-      </c>
-      <c r="B101">
-        <v>2017</v>
-      </c>
-      <c r="C101" t="s">
-        <v>50</v>
-      </c>
-      <c r="D101" t="s">
-        <v>10</v>
-      </c>
-      <c r="F101" t="s">
-        <v>112</v>
-      </c>
-      <c r="H101" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>7</v>
-      </c>
-      <c r="B102">
-        <v>2017</v>
-      </c>
-      <c r="C102" t="s">
-        <v>48</v>
-      </c>
-      <c r="D102" t="s">
-        <v>10</v>
-      </c>
-      <c r="F102" t="s">
-        <v>14</v>
-      </c>
-      <c r="H102" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>6</v>
-      </c>
-      <c r="B103">
-        <v>2017</v>
-      </c>
-      <c r="C103" t="s">
-        <v>48</v>
-      </c>
-      <c r="D103" t="s">
-        <v>10</v>
-      </c>
-      <c r="F103" t="s">
-        <v>27</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H103" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>73</v>
-      </c>
-      <c r="B104">
-        <v>2017</v>
-      </c>
-      <c r="C104" t="s">
-        <v>48</v>
-      </c>
-      <c r="D104" t="s">
-        <v>10</v>
-      </c>
-      <c r="F104" t="s">
-        <v>77</v>
+      <c r="D104" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="H104" t="s">
-        <v>75</v>
+        <v>204</v>
       </c>
     </row>
     <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
@@ -3240,6 +3243,7 @@
       <c r="F105" t="s">
         <v>14</v>
       </c>
+      <c r="G105" s="1"/>
       <c r="H105" t="s">
         <v>151</v>
       </c>
@@ -3260,6 +3264,7 @@
       <c r="F106" t="s">
         <v>181</v>
       </c>
+      <c r="G106" s="1"/>
       <c r="H106" t="s">
         <v>180</v>
       </c>
@@ -3277,6 +3282,7 @@
       <c r="D107" t="s">
         <v>16</v>
       </c>
+      <c r="G107" s="1"/>
       <c r="H107" t="s">
         <v>146</v>
       </c>
@@ -3297,36 +3303,40 @@
       <c r="F108" t="s">
         <v>43</v>
       </c>
+      <c r="G108" s="1"/>
       <c r="H108" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B109">
-        <v>2018</v>
+        <v>2002</v>
       </c>
       <c r="C109" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D109" t="s">
         <v>10</v>
       </c>
       <c r="F109" t="s">
-        <v>196</v>
-      </c>
-      <c r="H109" t="s">
-        <v>147</v>
+        <v>19</v>
+      </c>
+      <c r="G109" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H109" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B110">
-        <v>2018</v>
+        <v>2005</v>
       </c>
       <c r="C110" t="s">
         <v>48</v>
@@ -3335,10 +3345,13 @@
         <v>10</v>
       </c>
       <c r="F110" t="s">
-        <v>197</v>
-      </c>
-      <c r="H110" t="s">
-        <v>12</v>
+        <v>21</v>
+      </c>
+      <c r="G110" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
@@ -3357,6 +3370,7 @@
       <c r="F111" t="s">
         <v>148</v>
       </c>
+      <c r="G111" s="1"/>
       <c r="H111" t="s">
         <v>152</v>
       </c>
@@ -3377,6 +3391,7 @@
       <c r="F112" t="s">
         <v>154</v>
       </c>
+      <c r="G112" s="1"/>
       <c r="H112" t="s">
         <v>153</v>
       </c>
@@ -3394,36 +3409,40 @@
       <c r="D113" t="s">
         <v>16</v>
       </c>
+      <c r="G113" s="1"/>
       <c r="H113" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B114">
-        <v>2019</v>
+        <v>2008</v>
       </c>
       <c r="C114" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D114" t="s">
         <v>10</v>
       </c>
       <c r="F114" t="s">
-        <v>137</v>
+        <v>24</v>
+      </c>
+      <c r="G114" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="H114" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B115">
-        <v>2019</v>
+        <v>2011</v>
       </c>
       <c r="C115" t="s">
         <v>48</v>
@@ -3432,10 +3451,13 @@
         <v>10</v>
       </c>
       <c r="F115" t="s">
-        <v>42</v>
+        <v>25</v>
+      </c>
+      <c r="G115" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="H115" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
@@ -3454,6 +3476,7 @@
       <c r="F116" t="s">
         <v>137</v>
       </c>
+      <c r="G116" s="1"/>
       <c r="H116" t="s">
         <v>155</v>
       </c>
@@ -3474,6 +3497,7 @@
       <c r="F117" t="s">
         <v>137</v>
       </c>
+      <c r="G117" s="1"/>
       <c r="H117" t="s">
         <v>192</v>
       </c>
@@ -3511,6 +3535,7 @@
       <c r="F119" t="s">
         <v>119</v>
       </c>
+      <c r="G119" s="1"/>
       <c r="H119" t="s">
         <v>118</v>
       </c>
@@ -3531,6 +3556,7 @@
       <c r="F120" t="s">
         <v>37</v>
       </c>
+      <c r="G120" s="1"/>
       <c r="H120" t="s">
         <v>36</v>
       </c>
@@ -3551,68 +3577,78 @@
       <c r="F121" t="s">
         <v>78</v>
       </c>
+      <c r="G121" s="1"/>
       <c r="H121" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B122">
-        <v>2020</v>
+        <v>2014</v>
       </c>
       <c r="C122" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D122" t="s">
         <v>10</v>
       </c>
       <c r="F122" t="s">
-        <v>139</v>
+        <v>26</v>
+      </c>
+      <c r="G122" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="H122" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="B123">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="C123" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D123" t="s">
         <v>10</v>
       </c>
       <c r="F123" t="s">
-        <v>117</v>
+        <v>27</v>
+      </c>
+      <c r="G123" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="H123" t="s">
-        <v>116</v>
+        <v>35</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="B124">
-        <v>2020</v>
+        <v>2008</v>
       </c>
       <c r="C124" t="s">
-        <v>48</v>
+        <v>126</v>
       </c>
       <c r="D124" t="s">
-        <v>10</v>
+        <v>127</v>
       </c>
       <c r="F124" t="s">
-        <v>37</v>
-      </c>
-      <c r="H124" s="4" t="s">
-        <v>9</v>
+        <v>131</v>
+      </c>
+      <c r="G124" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="H124" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
@@ -3620,19 +3656,22 @@
         <v>73</v>
       </c>
       <c r="B125">
-        <v>2020</v>
+        <v>2008</v>
       </c>
       <c r="C125" t="s">
-        <v>48</v>
+        <v>126</v>
       </c>
       <c r="D125" t="s">
-        <v>10</v>
+        <v>127</v>
       </c>
       <c r="F125" t="s">
-        <v>78</v>
-      </c>
-      <c r="H125" t="s">
-        <v>74</v>
+        <v>131</v>
+      </c>
+      <c r="G125" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H125" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
@@ -3651,6 +3690,7 @@
       <c r="F126" t="s">
         <v>157</v>
       </c>
+      <c r="G126" s="1"/>
       <c r="H126" t="s">
         <v>156</v>
       </c>
@@ -3668,6 +3708,7 @@
       <c r="D127" t="s">
         <v>174</v>
       </c>
+      <c r="G127" s="1"/>
       <c r="H127" t="s">
         <v>182</v>
       </c>
@@ -3685,70 +3726,76 @@
       <c r="D128" t="s">
         <v>16</v>
       </c>
+      <c r="G128" s="1"/>
       <c r="H128" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B129" s="5">
+      <c r="A129" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B129" s="4">
         <v>2021</v>
       </c>
-      <c r="C129" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D129" s="5" t="s">
+      <c r="C129" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D129" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F129" t="s">
         <v>81</v>
       </c>
+      <c r="G129" s="1"/>
       <c r="H129" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="B130">
-        <v>2021</v>
+        <v>2008</v>
       </c>
       <c r="C130" t="s">
-        <v>50</v>
+        <v>126</v>
       </c>
       <c r="D130" t="s">
-        <v>10</v>
+        <v>127</v>
       </c>
       <c r="F130" t="s">
-        <v>81</v>
-      </c>
-      <c r="H130" t="s">
-        <v>140</v>
+        <v>131</v>
+      </c>
+      <c r="G130" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="H130" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A131" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B131" s="5">
-        <v>2021</v>
-      </c>
-      <c r="C131" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D131" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E131" s="5"/>
-      <c r="F131" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G131" s="6"/>
-      <c r="H131" s="5" t="s">
-        <v>85</v>
+      <c r="A131" t="s">
+        <v>73</v>
+      </c>
+      <c r="B131">
+        <v>2011</v>
+      </c>
+      <c r="C131" t="s">
+        <v>115</v>
+      </c>
+      <c r="D131" t="s">
+        <v>10</v>
+      </c>
+      <c r="F131" t="s">
+        <v>120</v>
+      </c>
+      <c r="G131" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H131" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
@@ -3767,6 +3814,7 @@
       <c r="F132" t="s">
         <v>81</v>
       </c>
+      <c r="G132" s="1"/>
       <c r="H132" t="s">
         <v>158</v>
       </c>
@@ -3784,72 +3832,74 @@
       <c r="D133" t="s">
         <v>16</v>
       </c>
+      <c r="G133" s="1"/>
       <c r="H133" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B134" s="5">
+      <c r="A134" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B134" s="4">
         <v>2022</v>
       </c>
-      <c r="C134" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D134" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E134" s="5"/>
-      <c r="F134" s="5" t="s">
+      <c r="C134" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D134" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E134" s="4"/>
+      <c r="F134" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G134" s="6"/>
-      <c r="H134" s="5" t="s">
+      <c r="G134" s="5"/>
+      <c r="H134" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="B135">
-        <v>2022</v>
+        <v>2011</v>
       </c>
       <c r="C135" t="s">
+        <v>115</v>
+      </c>
+      <c r="D135" t="s">
+        <v>10</v>
+      </c>
+      <c r="F135" t="s">
+        <v>120</v>
+      </c>
+      <c r="G135" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="H135" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>73</v>
+      </c>
+      <c r="B136">
+        <v>2014</v>
+      </c>
+      <c r="C136" t="s">
         <v>50</v>
       </c>
-      <c r="D135" t="s">
-        <v>10</v>
-      </c>
-      <c r="F135" t="s">
-        <v>83</v>
-      </c>
-      <c r="H135" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A136" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B136" s="5">
-        <v>2022</v>
-      </c>
-      <c r="C136" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D136" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E136" s="5"/>
-      <c r="F136" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G136" s="6"/>
-      <c r="H136" s="5" t="s">
-        <v>82</v>
+      <c r="D136" t="s">
+        <v>10</v>
+      </c>
+      <c r="F136" t="s">
+        <v>107</v>
+      </c>
+      <c r="H136" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
@@ -3868,8 +3918,149 @@
       <c r="F137" t="s">
         <v>83</v>
       </c>
+      <c r="G137" s="1"/>
       <c r="H137" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>73</v>
+      </c>
+      <c r="B138">
+        <v>2017</v>
+      </c>
+      <c r="C138" t="s">
+        <v>50</v>
+      </c>
+      <c r="D138" t="s">
+        <v>10</v>
+      </c>
+      <c r="F138" t="s">
+        <v>112</v>
+      </c>
+      <c r="H138" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>73</v>
+      </c>
+      <c r="B139">
+        <v>2020</v>
+      </c>
+      <c r="C139" t="s">
+        <v>50</v>
+      </c>
+      <c r="D139" t="s">
+        <v>10</v>
+      </c>
+      <c r="F139" t="s">
+        <v>117</v>
+      </c>
+      <c r="H139" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>73</v>
+      </c>
+      <c r="B140">
+        <v>2008</v>
+      </c>
+      <c r="C140" t="s">
+        <v>48</v>
+      </c>
+      <c r="D140" t="s">
+        <v>10</v>
+      </c>
+      <c r="F140" t="s">
+        <v>61</v>
+      </c>
+      <c r="H140" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>73</v>
+      </c>
+      <c r="B141">
+        <v>2011</v>
+      </c>
+      <c r="C141" t="s">
+        <v>48</v>
+      </c>
+      <c r="D141" t="s">
+        <v>10</v>
+      </c>
+      <c r="F141" t="s">
+        <v>120</v>
+      </c>
+      <c r="H141" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>73</v>
+      </c>
+      <c r="B142">
+        <v>2014</v>
+      </c>
+      <c r="C142" t="s">
+        <v>48</v>
+      </c>
+      <c r="D142" t="s">
+        <v>10</v>
+      </c>
+      <c r="F142" t="s">
+        <v>87</v>
+      </c>
+      <c r="H142" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>73</v>
+      </c>
+      <c r="B143">
+        <v>2017</v>
+      </c>
+      <c r="C143" t="s">
+        <v>48</v>
+      </c>
+      <c r="D143" t="s">
+        <v>10</v>
+      </c>
+      <c r="F143" t="s">
+        <v>77</v>
+      </c>
+      <c r="H143" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>73</v>
+      </c>
+      <c r="B144">
+        <v>2020</v>
+      </c>
+      <c r="C144" t="s">
+        <v>48</v>
+      </c>
+      <c r="D144" t="s">
+        <v>10</v>
+      </c>
+      <c r="F144" t="s">
+        <v>78</v>
+      </c>
+      <c r="H144" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3884,10 +4075,10 @@
       <sortCondition ref="B1:B137"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H137">
-    <sortCondition ref="A2:A137"/>
-    <sortCondition ref="D2:D137"/>
-    <sortCondition ref="C2:C137"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:H144">
+    <sortCondition ref="A2:A144"/>
+    <sortCondition ref="D2:D144"/>
+    <sortCondition ref="C2:C144"/>
   </sortState>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
@@ -3908,14 +4099,14 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="H8" r:id="rId1" xr:uid="{3A864FC9-E9A6-9E49-9148-BCE178E64C95}"/>
-    <hyperlink ref="H124" r:id="rId2" xr:uid="{2EBBCCD4-0AE8-344A-A3EC-2BED21CB47EE}"/>
+    <hyperlink ref="H87" r:id="rId2" xr:uid="{2EBBCCD4-0AE8-344A-A3EC-2BED21CB47EE}"/>
     <hyperlink ref="H75" r:id="rId3" xr:uid="{C2E4A6B9-5621-B549-B57E-A831E5A80B44}"/>
     <hyperlink ref="H49" r:id="rId4" xr:uid="{81E6D9E0-9F41-C14E-A9FE-A54BD14CE8DE}"/>
-    <hyperlink ref="H36" r:id="rId5" xr:uid="{73D76BFE-3329-E24F-BF51-6DE2D7EABDC5}"/>
-    <hyperlink ref="H37" r:id="rId6" xr:uid="{7CD351E3-780B-E34B-A618-1555BF35832E}"/>
-    <hyperlink ref="H11" r:id="rId7" xr:uid="{3B0CDB0E-607B-374B-9692-9E56E9B957D9}"/>
-    <hyperlink ref="H22" r:id="rId8" xr:uid="{24B7ED56-E7A5-A74B-A6D0-94A6A953612A}"/>
-    <hyperlink ref="H23" r:id="rId9" xr:uid="{9F3A0EC8-88EF-BA42-B2C4-CD63FAF3743E}"/>
+    <hyperlink ref="H125" r:id="rId5" xr:uid="{73D76BFE-3329-E24F-BF51-6DE2D7EABDC5}"/>
+    <hyperlink ref="H130" r:id="rId6" xr:uid="{7CD351E3-780B-E34B-A618-1555BF35832E}"/>
+    <hyperlink ref="H109" r:id="rId7" xr:uid="{3B0CDB0E-607B-374B-9692-9E56E9B957D9}"/>
+    <hyperlink ref="H110" r:id="rId8" xr:uid="{24B7ED56-E7A5-A74B-A6D0-94A6A953612A}"/>
+    <hyperlink ref="H53" r:id="rId9" xr:uid="{9F3A0EC8-88EF-BA42-B2C4-CD63FAF3743E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
increment/update epa downloads log
</commit_message>
<xml_diff>
--- a/_transportation/data-raw/epa/epa_downloads.xlsx
+++ b/_transportation/data-raw/epa/epa_downloads.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotenle/Documents/MetC_Locals/Interdivisional/ghg-cprg/_transportation/data-raw/epa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37F5ABF-C347-1D44-85DE-CD10D0F0E9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E696F8-B635-0641-8D52-6CC06C6F7851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="30720" windowHeight="17040" xr2:uid="{E3501ACA-8D46-AF4B-AC5D-95BB483C9130}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17040" xr2:uid="{E3501ACA-8D46-AF4B-AC5D-95BB483C9130}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="notes" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$I$146</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$I$157</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="259">
   <si>
     <t>file_name</t>
   </si>
@@ -349,9 +349,6 @@
     <t>https://gaftp.epa.gov/Air/emismod/2011/v3platform/2011emissions/2011ek_cb6v2_v6_11g_inputs_nonroad_part1.zip</t>
   </si>
   <si>
-    <t>2011ek_cb6v2_v6_11g</t>
-  </si>
-  <si>
     <t>https://gaftp.epa.gov/Air/emismod/2016/v3/2016emissions/2016gf_onroad_activity_15dec2022.zip</t>
   </si>
   <si>
@@ -788,6 +785,39 @@
   </si>
   <si>
     <t>2014NEI</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/air/emismod/2011/v3platform/2011emissions/2011ek_onroad_SMOKE_MOVES_MOVES2014a_forOTAQ_21jan2016_v2_AL_to_MO.zip</t>
+  </si>
+  <si>
+    <t>AL to MO</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/air/emismod/2011/v3platform/2011emissions/2011ek_onroad_SMOKE_MOVES_MOVES2014a_forOTAQ_21jan2016_v2_MT_to_WY.zip</t>
+  </si>
+  <si>
+    <t>MT to WY</t>
+  </si>
+  <si>
+    <t>2011ek</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/Air/nei/2017/doc/flat_files/2017NEI_onroad_20200427.zip</t>
+  </si>
+  <si>
+    <t>contains 2017NEI_onroad_CONUS_noCalifornia.csv</t>
+  </si>
+  <si>
+    <t>onroad by region</t>
+  </si>
+  <si>
+    <t>nonroad by region</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/air/emismod/2014/v2/2014fd/emissions/by_state/onroad/2014fd_onroad_FF10_SMOKE_MOVES2014a_FIPS_27.zip</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/air/emismod/2014/v2/2014fd/emissions/by_state/onroad/2014fd_onroad_FF10_SMOKE_MOVES2014a_FIPS_55.zip</t>
   </si>
 </sst>
 </file>
@@ -1338,10 +1368,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8EF959-18DF-BD43-B878-2D065289D72D}">
-  <dimension ref="A1:I155"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:I159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="123" workbookViewId="0">
-      <selection activeCell="A134" sqref="A134"/>
+    <sheetView tabSelected="1" zoomScale="123" workbookViewId="0">
+      <selection activeCell="G158" sqref="G158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1379,13 +1410,13 @@
         <v>1</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
@@ -1406,7 +1437,7 @@
       <c r="H2" s="8"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1425,13 +1456,13 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -1452,7 +1483,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1460,22 +1491,22 @@
         <v>2001</v>
       </c>
       <c r="C5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1490,17 +1521,17 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1518,7 +1549,7 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1536,7 +1567,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1554,13 +1585,13 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1568,20 +1599,20 @@
         <v>2002</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I10" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1598,13 +1629,13 @@
         <v>65</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -1612,22 +1643,22 @@
         <v>2002</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1647,13 +1678,13 @@
         <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1661,17 +1692,17 @@
         <v>2003</v>
       </c>
       <c r="C14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1689,7 +1720,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1707,7 +1738,7 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1715,17 +1746,17 @@
         <v>2004</v>
       </c>
       <c r="C17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1743,7 +1774,7 @@
       </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1761,7 +1792,7 @@
       </c>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1778,7 +1809,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1796,7 +1827,7 @@
       </c>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1814,13 +1845,13 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I22" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1828,23 +1859,23 @@
         <v>2005</v>
       </c>
       <c r="C23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I23" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1858,19 +1889,19 @@
         <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G24" t="s">
         <v>55</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1884,19 +1915,19 @@
         <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G25" t="s">
         <v>56</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I25" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>5</v>
       </c>
@@ -1904,22 +1935,22 @@
         <v>2005</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I26" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1939,13 +1970,13 @@
         <v>22</v>
       </c>
       <c r="H27" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1953,17 +1984,17 @@
         <v>2006</v>
       </c>
       <c r="C28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1981,7 +2012,7 @@
       </c>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1998,7 +2029,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -2006,17 +2037,17 @@
         <v>2007</v>
       </c>
       <c r="C31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -2030,11 +2061,11 @@
         <v>15</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -2051,7 +2082,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -2065,10 +2096,10 @@
         <v>9</v>
       </c>
       <c r="G34" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -2086,7 +2117,7 @@
       </c>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -2104,13 +2135,13 @@
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I36" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -2118,20 +2149,20 @@
         <v>2008</v>
       </c>
       <c r="C37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I37" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -2148,13 +2179,13 @@
         <v>60</v>
       </c>
       <c r="H38" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I38" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -2172,13 +2203,13 @@
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I39" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -2186,23 +2217,23 @@
         <v>2008</v>
       </c>
       <c r="C40" t="s">
+        <v>171</v>
+      </c>
+      <c r="D40" t="s">
         <v>172</v>
       </c>
-      <c r="D40" t="s">
-        <v>173</v>
-      </c>
       <c r="F40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I40" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -2210,25 +2241,25 @@
         <v>2008</v>
       </c>
       <c r="C41" t="s">
+        <v>124</v>
+      </c>
+      <c r="D41" t="s">
         <v>125</v>
       </c>
-      <c r="D41" t="s">
+      <c r="F41" t="s">
+        <v>129</v>
+      </c>
+      <c r="G41" t="s">
+        <v>130</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I41" t="s">
         <v>126</v>
       </c>
-      <c r="F41" t="s">
-        <v>130</v>
-      </c>
-      <c r="G41" t="s">
-        <v>131</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="I41" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>72</v>
       </c>
@@ -2236,25 +2267,25 @@
         <v>2008</v>
       </c>
       <c r="C42" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" t="s">
         <v>125</v>
       </c>
-      <c r="D42" t="s">
-        <v>126</v>
-      </c>
       <c r="F42" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -2262,25 +2293,25 @@
         <v>2008</v>
       </c>
       <c r="C43" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43" t="s">
         <v>125</v>
       </c>
-      <c r="D43" t="s">
-        <v>126</v>
-      </c>
       <c r="F43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -2297,13 +2328,13 @@
         <v>60</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I44" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>5</v>
       </c>
@@ -2311,22 +2342,22 @@
         <v>2008</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F45" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H45" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -2346,13 +2377,13 @@
         <v>27</v>
       </c>
       <c r="H46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I46" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -2360,17 +2391,17 @@
         <v>2009</v>
       </c>
       <c r="C47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -2388,7 +2419,7 @@
       </c>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -2405,7 +2436,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -2413,17 +2444,17 @@
         <v>2010</v>
       </c>
       <c r="C50" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -2441,7 +2472,7 @@
       </c>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -2458,7 +2489,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -2475,13 +2506,13 @@
         <v>52</v>
       </c>
       <c r="H53" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I53" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -2495,19 +2526,19 @@
         <v>15</v>
       </c>
       <c r="F54" t="s">
-        <v>102</v>
+        <v>252</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>100</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I54" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -2521,19 +2552,19 @@
         <v>15</v>
       </c>
       <c r="F55" t="s">
-        <v>102</v>
+        <v>252</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>98</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I55" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -2553,13 +2584,13 @@
         <v>56</v>
       </c>
       <c r="H56" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I56" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -2567,23 +2598,23 @@
         <v>2011</v>
       </c>
       <c r="C57" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D57" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F57" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I57" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -2603,13 +2634,13 @@
         <v>55</v>
       </c>
       <c r="H58" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I58" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>72</v>
       </c>
@@ -2623,17 +2654,17 @@
         <v>15</v>
       </c>
       <c r="F59" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I59" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -2651,13 +2682,13 @@
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I60" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>72</v>
       </c>
@@ -2665,23 +2696,23 @@
         <v>2011</v>
       </c>
       <c r="C61" t="s">
+        <v>171</v>
+      </c>
+      <c r="D61" t="s">
         <v>172</v>
       </c>
-      <c r="D61" t="s">
-        <v>173</v>
-      </c>
       <c r="F61" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I61" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>72</v>
       </c>
@@ -2689,25 +2720,25 @@
         <v>2011</v>
       </c>
       <c r="C62" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D62" t="s">
         <v>9</v>
       </c>
       <c r="F62" t="s">
+        <v>118</v>
+      </c>
+      <c r="G62" t="s">
+        <v>120</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I62" t="s">
         <v>119</v>
       </c>
-      <c r="G62" t="s">
-        <v>121</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="I62" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>72</v>
       </c>
@@ -2715,25 +2746,25 @@
         <v>2011</v>
       </c>
       <c r="C63" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D63" t="s">
         <v>9</v>
       </c>
       <c r="F63" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G63" t="s">
+        <v>121</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I63" t="s">
         <v>122</v>
       </c>
-      <c r="H63" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="I63" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>5</v>
       </c>
@@ -2741,22 +2772,22 @@
         <v>2011</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F64" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H64" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I64" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>72</v>
       </c>
@@ -2770,16 +2801,16 @@
         <v>9</v>
       </c>
       <c r="F65" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I65" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -2799,13 +2830,13 @@
         <v>28</v>
       </c>
       <c r="H66" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I66" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -2822,7 +2853,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -2840,7 +2871,7 @@
       </c>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -2848,17 +2879,17 @@
         <v>2012</v>
       </c>
       <c r="C69" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D69" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -2876,7 +2907,7 @@
       </c>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>6</v>
       </c>
@@ -2893,7 +2924,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -2910,7 +2941,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>6</v>
       </c>
@@ -2931,7 +2962,7 @@
       <c r="H73" s="5"/>
       <c r="I73" s="4"/>
     </row>
-    <row r="74" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -2949,7 +2980,7 @@
       </c>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -2966,7 +2997,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -2974,87 +3005,86 @@
         <v>2013</v>
       </c>
       <c r="C76" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D76" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="B77">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="C77" t="s">
-        <v>49</v>
+        <v>238</v>
       </c>
       <c r="D77" t="s">
         <v>9</v>
       </c>
       <c r="F77" t="s">
-        <v>94</v>
-      </c>
-      <c r="H77" t="s">
-        <v>210</v>
+        <v>252</v>
+      </c>
+      <c r="G77" t="s">
+        <v>249</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>205</v>
       </c>
       <c r="I77" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="B78">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="C78" t="s">
-        <v>47</v>
+        <v>238</v>
       </c>
       <c r="D78" t="s">
         <v>9</v>
       </c>
-      <c r="F78" t="s">
-        <v>40</v>
-      </c>
-      <c r="H78" t="s">
-        <v>210</v>
+      <c r="G78" t="s">
+        <v>251</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>205</v>
       </c>
       <c r="I78" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B79" s="4">
-        <v>2014</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F79" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G79" s="1"/>
-      <c r="H79" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="I79" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>72</v>
+      </c>
+      <c r="B79">
+        <v>2011</v>
+      </c>
+      <c r="C79" t="s">
+        <v>238</v>
+      </c>
+      <c r="D79" t="s">
+        <v>15</v>
+      </c>
+      <c r="F79" t="s">
+        <v>97</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -3062,23 +3092,22 @@
         <v>2014</v>
       </c>
       <c r="C80" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D80" t="s">
-        <v>15</v>
-      </c>
-      <c r="F80" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" t="s">
         <v>94</v>
       </c>
-      <c r="G80" s="1"/>
-      <c r="H80" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="I80" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="H80" t="s">
+        <v>209</v>
+      </c>
+      <c r="I80" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>6</v>
       </c>
@@ -3086,42 +3115,48 @@
         <v>2014</v>
       </c>
       <c r="C81" t="s">
-        <v>172</v>
+        <v>47</v>
       </c>
       <c r="D81" t="s">
-        <v>149</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H81" s="1"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="F81" t="s">
+        <v>40</v>
+      </c>
+      <c r="H81" t="s">
+        <v>209</v>
+      </c>
+      <c r="I81" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B82" s="4">
         <v>2014</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>114</v>
+        <v>49</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F82" t="s">
-        <v>236</v>
-      </c>
-      <c r="H82" t="s">
-        <v>229</v>
-      </c>
-      <c r="I82" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G82" s="1"/>
+      <c r="H82" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="I82" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B83">
         <v>2014</v>
@@ -3130,72 +3165,63 @@
         <v>47</v>
       </c>
       <c r="D83" t="s">
-        <v>9</v>
-      </c>
-      <c r="F83" t="s">
-        <v>25</v>
-      </c>
-      <c r="G83" t="s">
-        <v>29</v>
-      </c>
-      <c r="H83" t="s">
-        <v>229</v>
-      </c>
-      <c r="I83" t="s">
-        <v>33</v>
+        <v>15</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G83" s="1"/>
+      <c r="H83" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>72</v>
+        <v>6</v>
       </c>
       <c r="B84">
         <v>2014</v>
       </c>
       <c r="C84" t="s">
-        <v>114</v>
+        <v>171</v>
       </c>
       <c r="D84" t="s">
-        <v>15</v>
-      </c>
-      <c r="F84" t="s">
-        <v>108</v>
-      </c>
-      <c r="G84" s="1"/>
-      <c r="H84" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="I84" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>72</v>
-      </c>
-      <c r="B85">
+        <v>148</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H84" s="1"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85" s="4">
         <v>2014</v>
       </c>
-      <c r="C85" t="s">
-        <v>114</v>
-      </c>
-      <c r="D85" t="s">
-        <v>15</v>
+      <c r="C85" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="F85" t="s">
-        <v>106</v>
-      </c>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1" t="s">
-        <v>221</v>
+        <v>235</v>
+      </c>
+      <c r="H85" t="s">
+        <v>228</v>
       </c>
       <c r="I85" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="B86">
         <v>2014</v>
@@ -3204,17 +3230,19 @@
         <v>47</v>
       </c>
       <c r="D86" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F86" t="s">
-        <v>86</v>
-      </c>
-      <c r="G86" s="1"/>
-      <c r="H86" s="1" t="s">
-        <v>221</v>
+        <v>25</v>
+      </c>
+      <c r="G86" t="s">
+        <v>29</v>
+      </c>
+      <c r="H86" t="s">
+        <v>228</v>
       </c>
       <c r="I86" t="s">
-        <v>87</v>
+        <v>33</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3225,20 +3253,20 @@
         <v>2014</v>
       </c>
       <c r="C87" t="s">
-        <v>172</v>
+        <v>113</v>
       </c>
       <c r="D87" t="s">
-        <v>173</v>
+        <v>15</v>
       </c>
       <c r="F87" t="s">
-        <v>177</v>
+        <v>107</v>
       </c>
       <c r="G87" s="1"/>
       <c r="H87" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I87" t="s">
-        <v>175</v>
+        <v>106</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3249,19 +3277,20 @@
         <v>2014</v>
       </c>
       <c r="C88" t="s">
-        <v>49</v>
+        <v>113</v>
       </c>
       <c r="D88" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F88" t="s">
-        <v>106</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="G88" s="1"/>
       <c r="H88" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I88" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3275,19 +3304,20 @@
         <v>47</v>
       </c>
       <c r="D89" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F89" t="s">
         <v>86</v>
       </c>
+      <c r="G89" s="1"/>
       <c r="H89" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I89" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>6</v>
       </c>
@@ -3304,13 +3334,13 @@
         <v>37</v>
       </c>
       <c r="H90" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I90" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>6</v>
       </c>
@@ -3327,16 +3357,16 @@
         <v>37</v>
       </c>
       <c r="G91" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H91" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I91" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -3353,13 +3383,13 @@
         <v>37</v>
       </c>
       <c r="H92" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I92" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -3377,13 +3407,13 @@
       </c>
       <c r="G93" s="1"/>
       <c r="H93" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I93" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>6</v>
       </c>
@@ -3397,12 +3427,12 @@
         <v>15</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H94" s="1"/>
       <c r="I94" s="3"/>
     </row>
-    <row r="95" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -3410,20 +3440,20 @@
         <v>2015</v>
       </c>
       <c r="C95" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D95" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G95" s="1"/>
       <c r="H95" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I95" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -3437,16 +3467,16 @@
         <v>9</v>
       </c>
       <c r="F96" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H96" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I96" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>6</v>
       </c>
@@ -3463,13 +3493,13 @@
         <v>43</v>
       </c>
       <c r="H97" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I97" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>6</v>
       </c>
@@ -3477,23 +3507,23 @@
         <v>2016</v>
       </c>
       <c r="C98" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D98" t="s">
         <v>15</v>
       </c>
       <c r="F98" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G98" s="1"/>
       <c r="H98" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I98" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>6</v>
       </c>
@@ -3507,17 +3537,17 @@
         <v>15</v>
       </c>
       <c r="F99" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G99" s="1"/>
       <c r="H99" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I99" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>6</v>
       </c>
@@ -3525,20 +3555,20 @@
         <v>2016</v>
       </c>
       <c r="C100" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D100" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G100" s="1"/>
       <c r="H100" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I100" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>6</v>
       </c>
@@ -3555,13 +3585,13 @@
         <v>13</v>
       </c>
       <c r="H101" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I101" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>6</v>
       </c>
@@ -3578,13 +3608,13 @@
         <v>13</v>
       </c>
       <c r="H102" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I102" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>6</v>
       </c>
@@ -3602,7 +3632,7 @@
       </c>
       <c r="H103" s="1"/>
     </row>
-    <row r="104" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>6</v>
       </c>
@@ -3620,13 +3650,13 @@
       </c>
       <c r="G104" s="1"/>
       <c r="H104" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I104" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -3634,23 +3664,23 @@
         <v>2017</v>
       </c>
       <c r="C105" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D105" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F105" t="s">
         <v>13</v>
       </c>
       <c r="G105" s="1"/>
       <c r="H105" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I105" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>5</v>
       </c>
@@ -3658,22 +3688,22 @@
         <v>2017</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F106" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H106" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I106" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>5</v>
       </c>
@@ -3690,13 +3720,13 @@
         <v>26</v>
       </c>
       <c r="H107" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I107" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>5</v>
       </c>
@@ -3716,13 +3746,13 @@
         <v>30</v>
       </c>
       <c r="H108" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I108" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>72</v>
       </c>
@@ -3730,23 +3760,23 @@
         <v>2017</v>
       </c>
       <c r="C109" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D109" t="s">
         <v>15</v>
       </c>
       <c r="F109" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G109" s="1"/>
       <c r="H109" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I109" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>72</v>
       </c>
@@ -3762,15 +3792,17 @@
       <c r="F110" t="s">
         <v>76</v>
       </c>
-      <c r="G110" s="1"/>
+      <c r="G110" s="1" t="s">
+        <v>256</v>
+      </c>
       <c r="H110" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I110" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>72</v>
       </c>
@@ -3778,23 +3810,23 @@
         <v>2017</v>
       </c>
       <c r="C111" t="s">
+        <v>171</v>
+      </c>
+      <c r="D111" t="s">
         <v>172</v>
       </c>
-      <c r="D111" t="s">
-        <v>173</v>
-      </c>
       <c r="F111" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G111" s="1"/>
       <c r="H111" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I111" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>72</v>
       </c>
@@ -3808,16 +3840,16 @@
         <v>9</v>
       </c>
       <c r="F112" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I112" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>72</v>
       </c>
@@ -3833,14 +3865,17 @@
       <c r="F113" t="s">
         <v>76</v>
       </c>
+      <c r="G113" t="s">
+        <v>255</v>
+      </c>
       <c r="H113" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I113" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -3854,16 +3889,16 @@
         <v>9</v>
       </c>
       <c r="F114" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H114" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I114" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>6</v>
       </c>
@@ -3877,16 +3912,16 @@
         <v>9</v>
       </c>
       <c r="F115" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H115" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I115" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>6</v>
       </c>
@@ -3894,20 +3929,20 @@
         <v>2018</v>
       </c>
       <c r="C116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D116" t="s">
         <v>15</v>
       </c>
       <c r="G116" s="1"/>
       <c r="H116" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I116" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>6</v>
       </c>
@@ -3925,13 +3960,13 @@
       </c>
       <c r="G117" s="1"/>
       <c r="H117" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I117" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>6</v>
       </c>
@@ -3939,23 +3974,23 @@
         <v>2018</v>
       </c>
       <c r="C118" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D118" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F118" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G118" s="1"/>
       <c r="H118" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I118" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>6</v>
       </c>
@@ -3963,23 +3998,23 @@
         <v>2018</v>
       </c>
       <c r="C119" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D119" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F119" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G119" s="1"/>
       <c r="H119" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I119" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>6</v>
       </c>
@@ -3993,16 +4028,16 @@
         <v>9</v>
       </c>
       <c r="F120" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H120" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I120" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>6</v>
       </c>
@@ -4019,13 +4054,13 @@
         <v>41</v>
       </c>
       <c r="H121" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I121" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>6</v>
       </c>
@@ -4033,20 +4068,20 @@
         <v>2019</v>
       </c>
       <c r="C122" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D122" t="s">
         <v>15</v>
       </c>
       <c r="G122" s="1"/>
       <c r="H122" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I122" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>6</v>
       </c>
@@ -4054,23 +4089,23 @@
         <v>2019</v>
       </c>
       <c r="C123" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D123" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F123" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G123" s="1"/>
       <c r="H123" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I123" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>6</v>
       </c>
@@ -4084,17 +4119,17 @@
         <v>15</v>
       </c>
       <c r="F124" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G124" s="1"/>
       <c r="H124" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I124" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>6</v>
       </c>
@@ -4108,16 +4143,16 @@
         <v>9</v>
       </c>
       <c r="F125" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H125" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I125" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>6</v>
       </c>
@@ -4134,13 +4169,13 @@
         <v>36</v>
       </c>
       <c r="H126" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I126" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>6</v>
       </c>
@@ -4148,7 +4183,7 @@
         <v>2020</v>
       </c>
       <c r="C127" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D127" t="s">
         <v>15</v>
@@ -4158,7 +4193,7 @@
       </c>
       <c r="H127" s="8"/>
     </row>
-    <row r="128" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>6</v>
       </c>
@@ -4176,13 +4211,13 @@
       </c>
       <c r="G128" s="1"/>
       <c r="H128" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I128" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>6</v>
       </c>
@@ -4190,23 +4225,23 @@
         <v>2020</v>
       </c>
       <c r="C129" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D129" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F129" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G129" s="1"/>
       <c r="H129" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I129" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>72</v>
       </c>
@@ -4214,23 +4249,23 @@
         <v>2020</v>
       </c>
       <c r="C130" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D130" t="s">
         <v>15</v>
       </c>
       <c r="F130" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G130" s="1"/>
       <c r="H130" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I130" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>72</v>
       </c>
@@ -4248,13 +4283,13 @@
       </c>
       <c r="G131" s="1"/>
       <c r="H131" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I131" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>72</v>
       </c>
@@ -4262,20 +4297,20 @@
         <v>2020</v>
       </c>
       <c r="C132" t="s">
+        <v>171</v>
+      </c>
+      <c r="D132" t="s">
         <v>172</v>
-      </c>
-      <c r="D132" t="s">
-        <v>173</v>
       </c>
       <c r="G132" s="1"/>
       <c r="H132" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I132" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>72</v>
       </c>
@@ -4289,16 +4324,16 @@
         <v>9</v>
       </c>
       <c r="F133" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I133" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>72</v>
       </c>
@@ -4306,22 +4341,22 @@
         <v>2020</v>
       </c>
       <c r="C134" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D134" t="s">
         <v>9</v>
       </c>
       <c r="F134" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H134" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I134" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>72</v>
       </c>
@@ -4329,22 +4364,22 @@
         <v>2020</v>
       </c>
       <c r="C135" t="s">
+        <v>238</v>
+      </c>
+      <c r="D135" t="s">
+        <v>15</v>
+      </c>
+      <c r="F135" t="s">
+        <v>115</v>
+      </c>
+      <c r="H135" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I135" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="D135" t="s">
-        <v>15</v>
-      </c>
-      <c r="F135" t="s">
-        <v>116</v>
-      </c>
-      <c r="H135" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="I135" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="136" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>72</v>
       </c>
@@ -4361,13 +4396,13 @@
         <v>77</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I136" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>6</v>
       </c>
@@ -4384,13 +4419,13 @@
         <v>80</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I137" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>6</v>
       </c>
@@ -4409,13 +4444,13 @@
       </c>
       <c r="G138" s="4"/>
       <c r="H138" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I138" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>6</v>
       </c>
@@ -4423,20 +4458,20 @@
         <v>2021</v>
       </c>
       <c r="C139" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D139" t="s">
         <v>15</v>
       </c>
       <c r="G139" s="1"/>
       <c r="H139" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I139" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>6</v>
       </c>
@@ -4454,13 +4489,13 @@
       </c>
       <c r="G140" s="1"/>
       <c r="H140" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I140" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>6</v>
       </c>
@@ -4468,23 +4503,23 @@
         <v>2021</v>
       </c>
       <c r="C141" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D141" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F141" t="s">
         <v>80</v>
       </c>
       <c r="G141" s="1"/>
       <c r="H141" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I141" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>6</v>
       </c>
@@ -4501,13 +4536,13 @@
         <v>82</v>
       </c>
       <c r="H142" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I142" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>6</v>
       </c>
@@ -4526,13 +4561,13 @@
       </c>
       <c r="G143" s="4"/>
       <c r="H143" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I143" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>6</v>
       </c>
@@ -4540,20 +4575,20 @@
         <v>2022</v>
       </c>
       <c r="C144" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D144" t="s">
         <v>15</v>
       </c>
       <c r="G144" s="1"/>
       <c r="H144" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I144" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>6</v>
       </c>
@@ -4572,13 +4607,13 @@
       </c>
       <c r="G145" s="5"/>
       <c r="H145" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I145" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="146" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>6</v>
       </c>
@@ -4586,23 +4621,23 @@
         <v>2022</v>
       </c>
       <c r="C146" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D146" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F146" t="s">
         <v>82</v>
       </c>
       <c r="G146" s="1"/>
       <c r="H146" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I146" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>72</v>
       </c>
@@ -4610,25 +4645,25 @@
         <v>2017</v>
       </c>
       <c r="C147" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D147" t="s">
         <v>9</v>
       </c>
       <c r="F147" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G147" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H147" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I147" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>72</v>
       </c>
@@ -4636,25 +4671,25 @@
         <v>2017</v>
       </c>
       <c r="C148" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D148" t="s">
         <v>9</v>
       </c>
       <c r="F148" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G148" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H148" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I148" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>72</v>
       </c>
@@ -4662,19 +4697,19 @@
         <v>2017</v>
       </c>
       <c r="C149" t="s">
-        <v>239</v>
+        <v>47</v>
       </c>
       <c r="D149" t="s">
         <v>15</v>
       </c>
       <c r="F149" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H149" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I149" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="150" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4685,19 +4720,20 @@
         <v>2014</v>
       </c>
       <c r="C150" t="s">
-        <v>239</v>
+        <v>171</v>
       </c>
       <c r="D150" t="s">
-        <v>9</v>
+        <v>172</v>
       </c>
       <c r="F150" t="s">
-        <v>248</v>
-      </c>
-      <c r="H150" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="I150" s="3" t="s">
-        <v>242</v>
+        <v>176</v>
+      </c>
+      <c r="G150" s="1"/>
+      <c r="H150" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I150" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4708,19 +4744,19 @@
         <v>2014</v>
       </c>
       <c r="C151" t="s">
-        <v>239</v>
+        <v>49</v>
       </c>
       <c r="D151" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F151" t="s">
-        <v>248</v>
-      </c>
-      <c r="H151" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="I151" s="3" t="s">
-        <v>241</v>
+        <v>105</v>
+      </c>
+      <c r="H151" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I151" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4728,19 +4764,22 @@
         <v>72</v>
       </c>
       <c r="B152">
-        <v>2011</v>
+        <v>2014</v>
       </c>
       <c r="C152" t="s">
-        <v>239</v>
+        <v>47</v>
       </c>
       <c r="D152" t="s">
         <v>9</v>
       </c>
       <c r="F152" t="s">
-        <v>97</v>
-      </c>
-      <c r="H152" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H152" s="1" t="s">
         <v>220</v>
+      </c>
+      <c r="I152" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="153" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4748,19 +4787,22 @@
         <v>72</v>
       </c>
       <c r="B153">
-        <v>2011</v>
+        <v>2014</v>
       </c>
       <c r="C153" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D153" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F153" t="s">
-        <v>97</v>
+        <v>247</v>
       </c>
       <c r="H153" s="5" t="s">
         <v>220</v>
+      </c>
+      <c r="I153" s="3" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4768,25 +4810,25 @@
         <v>72</v>
       </c>
       <c r="B154">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="C154" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D154" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F154" t="s">
-        <v>60</v>
+        <v>247</v>
       </c>
       <c r="H154" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="I154" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+      <c r="I154" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>72</v>
       </c>
@@ -4794,25 +4836,131 @@
         <v>2008</v>
       </c>
       <c r="C155" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D155" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F155" t="s">
         <v>60</v>
       </c>
       <c r="H155" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I155" t="s">
-        <v>245</v>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>72</v>
+      </c>
+      <c r="B156">
+        <v>2008</v>
+      </c>
+      <c r="C156" t="s">
+        <v>238</v>
+      </c>
+      <c r="D156" t="s">
+        <v>15</v>
+      </c>
+      <c r="F156" t="s">
+        <v>60</v>
+      </c>
+      <c r="H156" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="I156" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>72</v>
+      </c>
+      <c r="B157">
+        <v>2017</v>
+      </c>
+      <c r="C157" t="s">
+        <v>47</v>
+      </c>
+      <c r="D157" t="s">
+        <v>9</v>
+      </c>
+      <c r="F157" t="s">
+        <v>110</v>
+      </c>
+      <c r="G157" t="s">
+        <v>254</v>
+      </c>
+      <c r="H157" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="I157" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>6</v>
+      </c>
+      <c r="B158">
+        <v>2014</v>
+      </c>
+      <c r="C158" t="s">
+        <v>238</v>
+      </c>
+      <c r="D158" t="s">
+        <v>9</v>
+      </c>
+      <c r="F158" t="s">
+        <v>94</v>
+      </c>
+      <c r="G158" t="s">
+        <v>120</v>
+      </c>
+      <c r="H158" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="I158" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>6</v>
+      </c>
+      <c r="B159">
+        <v>2014</v>
+      </c>
+      <c r="C159" t="s">
+        <v>238</v>
+      </c>
+      <c r="D159" t="s">
+        <v>9</v>
+      </c>
+      <c r="F159" t="s">
+        <v>94</v>
+      </c>
+      <c r="G159" t="s">
+        <v>121</v>
+      </c>
+      <c r="H159" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="I159" s="3" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I146" xr:uid="{EB8EF959-18DF-BD43-B878-2D065289D72D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I146">
-      <sortCondition ref="B1:B146"/>
+  <autoFilter ref="A1:I157" xr:uid="{EB8EF959-18DF-BD43-B878-2D065289D72D}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="2014"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A53:I154">
+      <sortCondition ref="B1:B156"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:I146">
@@ -4841,17 +4989,18 @@
   <hyperlinks>
     <hyperlink ref="I9" r:id="rId1" xr:uid="{3A864FC9-E9A6-9E49-9148-BCE178E64C95}"/>
     <hyperlink ref="I126" r:id="rId2" xr:uid="{2EBBCCD4-0AE8-344A-A3EC-2BED21CB47EE}"/>
-    <hyperlink ref="I79" r:id="rId3" xr:uid="{C2E4A6B9-5621-B549-B57E-A831E5A80B44}"/>
+    <hyperlink ref="I82" r:id="rId3" xr:uid="{C2E4A6B9-5621-B549-B57E-A831E5A80B44}"/>
     <hyperlink ref="I55" r:id="rId4" xr:uid="{81E6D9E0-9F41-C14E-A9FE-A54BD14CE8DE}"/>
     <hyperlink ref="I42" r:id="rId5" xr:uid="{73D76BFE-3329-E24F-BF51-6DE2D7EABDC5}"/>
     <hyperlink ref="I43" r:id="rId6" xr:uid="{7CD351E3-780B-E34B-A618-1555BF35832E}"/>
     <hyperlink ref="I13" r:id="rId7" xr:uid="{3B0CDB0E-607B-374B-9692-9E56E9B957D9}"/>
     <hyperlink ref="I27" r:id="rId8" xr:uid="{24B7ED56-E7A5-A74B-A6D0-94A6A953612A}"/>
     <hyperlink ref="I24" r:id="rId9" xr:uid="{9F3A0EC8-88EF-BA42-B2C4-CD63FAF3743E}"/>
-    <hyperlink ref="I80" r:id="rId10" xr:uid="{89E45E83-4EF9-8B44-AACC-ED2D2E60F75C}"/>
+    <hyperlink ref="I83" r:id="rId10" xr:uid="{89E45E83-4EF9-8B44-AACC-ED2D2E60F75C}"/>
     <hyperlink ref="I135" r:id="rId11" xr:uid="{FA8A1007-708D-DF45-A09D-78C317607EA1}"/>
-    <hyperlink ref="I150" r:id="rId12" xr:uid="{8AB8E0D9-B2E6-7A4B-B7FD-383AE4C17BF2}"/>
-    <hyperlink ref="I151" r:id="rId13" xr:uid="{6702C906-A8EA-954F-8C17-7147195B6C53}"/>
+    <hyperlink ref="I153" r:id="rId12" xr:uid="{8AB8E0D9-B2E6-7A4B-B7FD-383AE4C17BF2}"/>
+    <hyperlink ref="I154" r:id="rId13" xr:uid="{6702C906-A8EA-954F-8C17-7147195B6C53}"/>
+    <hyperlink ref="I159" r:id="rId14" xr:uid="{AFDA6783-AFA0-A040-820E-4E25136EB298}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4876,7 +5025,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -4884,7 +5033,7 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -4892,7 +5041,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -4900,7 +5049,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -4920,32 +5069,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update download log and documentation
</commit_message>
<xml_diff>
--- a/_transportation/data-raw/epa/epa_downloads.xlsx
+++ b/_transportation/data-raw/epa/epa_downloads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotenle/Documents/MetC_Locals/Interdivisional/ghg-cprg/_transportation/data-raw/epa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E696F8-B635-0641-8D52-6CC06C6F7851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC2E5F8-BEA8-434F-B359-384BF37BB24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17040" xr2:uid="{E3501ACA-8D46-AF4B-AC5D-95BB483C9130}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="261">
   <si>
     <t>file_name</t>
   </si>
@@ -818,6 +818,12 @@
   </si>
   <si>
     <t>https://gaftp.epa.gov/air/emismod/2014/v2/2014fd/emissions/by_state/onroad/2014fd_onroad_FF10_SMOKE_MOVES2014a_FIPS_55.zip</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/air/nei/2014/data_summaries/2014v2/CO_CO2_2014fd_nata_onroad_SMOKE_MOVES_MOVES2014a_forNATA_12jan2018_v1.zip</t>
+  </si>
+  <si>
+    <t>CO and CO2</t>
   </si>
 </sst>
 </file>
@@ -1369,10 +1375,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8EF959-18DF-BD43-B878-2D065289D72D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I159"/>
+  <dimension ref="A1:I160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="123" workbookViewId="0">
-      <selection activeCell="G158" sqref="G158"/>
+      <selection activeCell="A160" sqref="A160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4950,6 +4956,32 @@
       </c>
       <c r="I159" s="3" t="s">
         <v>258</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>72</v>
+      </c>
+      <c r="B160">
+        <v>2014</v>
+      </c>
+      <c r="C160" t="s">
+        <v>238</v>
+      </c>
+      <c r="D160" t="s">
+        <v>9</v>
+      </c>
+      <c r="F160" t="s">
+        <v>94</v>
+      </c>
+      <c r="G160" t="s">
+        <v>260</v>
+      </c>
+      <c r="H160" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="I160" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add direct CMAS data warehouse download links
</commit_message>
<xml_diff>
--- a/_transportation/data-raw/epa/epa_downloads.xlsx
+++ b/_transportation/data-raw/epa/epa_downloads.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotenle/Documents/MetC_Locals/Interdivisional/ghg-cprg/_transportation/data-raw/epa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC2E5F8-BEA8-434F-B359-384BF37BB24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2071D58-B675-8745-AAF0-8B08061C5EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17040" xr2:uid="{E3501ACA-8D46-AF4B-AC5D-95BB483C9130}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="30720" windowHeight="17040" xr2:uid="{E3501ACA-8D46-AF4B-AC5D-95BB483C9130}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="273">
   <si>
     <t>file_name</t>
   </si>
@@ -824,6 +824,42 @@
   </si>
   <si>
     <t>CO and CO2</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1jw_0216cTDSw-FrojrgGbKU5myl23ybv&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=fccfb764-8849-44fc-b506-7de81bbdd4e8&amp;at=AO7h07e29Tc-CjdVA7IphIHXaT1L:1727277124697</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1W1QBtNB89FfWdSE3RQdnFoedwjgn0ctB&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=9768171e-056f-45b5-aba8-71f4a69146dc&amp;at=AO7h07eZwuW4OJnGLz83u0LU7rHi:1727277818221</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1Y6D0YJuMy97hlhG58R5LjmVrVqucNlgy&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=0bf155e4-d9e9-44a9-ab43-8d93505a6b9b&amp;at=AO7h07eoLdEncM7sZJSEMmhw7bBE:1727277879290</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1TTzPa0vse1_z0On-82uBF53IQ6zY5DIX&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=33810c7d-2a28-4d52-bfc2-68598662f428&amp;at=AO7h07cwKOMiDUnr7tirwMaGCb8t:1727277945324</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1QIaSG3kyReCLUJXXgHubUZKuo1Q5pAsl&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=348fa232-1e5b-445c-9c37-5b49be9819ae&amp;at=AO7h07e7A3qXQiUtgm2L4-zYU3Io:1727277967596</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1ZCAzfSxfzehgKT3RdDO3K6MOko8heOii&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=e597b786-efbb-4922-8161-0af94006d6f0&amp;at=AO7h07cjDkT1iJ9hgSwJ7nIxUY1V:1727277988258</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=17qLqwJllqX-XloScSNaxdviQDspTufep&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=d6b82ccf-f5c3-41d2-9b2b-b7bfbf731eeb&amp;at=AO7h07cjoWUwZU0ju9kc4N35ZFQ6:1727278302203</t>
+  </si>
+  <si>
+    <t>_transportation/data-raw/epa/air_emissions_modeling/EQUATES/CMAS_Data_Warehouse</t>
+  </si>
+  <si>
+    <t>Contains N2O</t>
+  </si>
+  <si>
+    <t>EQUATES CMAS Data Warehouse</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1G2_LBLy7_n91Ur0ulsLZ9zwGs3luTzn2</t>
+  </si>
+  <si>
+    <t>Data downloaded from the CMAS Data Warehouse Google Drive includes many more sectors and scripts.</t>
   </si>
 </sst>
 </file>
@@ -1375,10 +1411,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8EF959-18DF-BD43-B878-2D065289D72D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I160"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="123" workbookViewId="0">
-      <selection activeCell="A160" sqref="A160"/>
+      <selection activeCell="C161" sqref="C161:C167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1389,7 +1425,7 @@
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="22.5" customWidth="1"/>
-    <col min="8" max="8" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="85.5" customWidth="1"/>
     <col min="9" max="9" width="115.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4982,6 +5018,149 @@
       </c>
       <c r="I160" t="s">
         <v>259</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>5</v>
+      </c>
+      <c r="B161">
+        <v>2002</v>
+      </c>
+      <c r="C161" t="s">
+        <v>238</v>
+      </c>
+      <c r="D161" t="s">
+        <v>9</v>
+      </c>
+      <c r="H161" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I161" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>5</v>
+      </c>
+      <c r="B162">
+        <v>2005</v>
+      </c>
+      <c r="C162" t="s">
+        <v>238</v>
+      </c>
+      <c r="D162" t="s">
+        <v>9</v>
+      </c>
+      <c r="H162" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I162" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>5</v>
+      </c>
+      <c r="B163">
+        <v>2008</v>
+      </c>
+      <c r="C163" t="s">
+        <v>238</v>
+      </c>
+      <c r="D163" t="s">
+        <v>9</v>
+      </c>
+      <c r="H163" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I163" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>5</v>
+      </c>
+      <c r="B164">
+        <v>2011</v>
+      </c>
+      <c r="C164" t="s">
+        <v>238</v>
+      </c>
+      <c r="D164" t="s">
+        <v>9</v>
+      </c>
+      <c r="H164" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I164" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>5</v>
+      </c>
+      <c r="B165">
+        <v>2014</v>
+      </c>
+      <c r="C165" t="s">
+        <v>238</v>
+      </c>
+      <c r="D165" t="s">
+        <v>9</v>
+      </c>
+      <c r="H165" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I165" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>5</v>
+      </c>
+      <c r="B166">
+        <v>2017</v>
+      </c>
+      <c r="C166" t="s">
+        <v>238</v>
+      </c>
+      <c r="D166" t="s">
+        <v>9</v>
+      </c>
+      <c r="H166" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I166" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>5</v>
+      </c>
+      <c r="B167">
+        <v>2019</v>
+      </c>
+      <c r="C167" t="s">
+        <v>238</v>
+      </c>
+      <c r="D167" t="s">
+        <v>9</v>
+      </c>
+      <c r="G167" t="s">
+        <v>269</v>
+      </c>
+      <c r="H167" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I167" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -5040,10 +5219,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D232C1-B777-0648-8306-8752ED74FD38}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="132" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5084,6 +5263,14 @@
         <v>186</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B5" t="s">
+        <v>271</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5091,10 +5278,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD660B9-EDB1-794A-9EA6-28DC0455076C}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5129,6 +5316,11 @@
         <v>234</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>272</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update downloads log; re-run readme
</commit_message>
<xml_diff>
--- a/_transportation/data-raw/epa/epa_downloads.xlsx
+++ b/_transportation/data-raw/epa/epa_downloads.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotenle/Documents/MetC_Locals/Interdivisional/ghg-cprg/_transportation/data-raw/epa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600726E5-911E-E348-8159-EA60B0810172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E9F250-9FE9-CF4B-AD29-FCE3F285C282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="30720" windowHeight="17040" xr2:uid="{E3501ACA-8D46-AF4B-AC5D-95BB483C9130}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17040" xr2:uid="{E3501ACA-8D46-AF4B-AC5D-95BB483C9130}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="317">
   <si>
     <t>file_name</t>
   </si>
@@ -860,13 +860,145 @@
   </si>
   <si>
     <t>Data downloaded from the CMAS Data Warehouse Google Drive includes many more sectors and scripts.</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1eSgTweGuX3xdP1ZZioyNufgHmmooPOcG&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=971b95d9-b965-44c9-b91a-6f3436495f86&amp;at=AN_67v2yl5IR2QHPYuNd5Gxsv9y-:1727793725340</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1r3B4TIKy5cestvKygL-2IMRD6OIq47XD&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=2a280431-7bdc-428a-963f-ddf0703dac60&amp;at=AN_67v2ascXZJsERRs76veVFW1-L:1727793829937</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1o1JpcQFMfgGZtE5EJpd5K9Aaj0E2EQso&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=f72e8f04-4107-4579-8d9a-c28f8984147b&amp;at=AN_67v0wITHCuhqWPNOHXGD-Lnoq:1727793840527</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1N4Gsoi6mZWzsawyZiRAgtpB53w27IyIl&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=a7749fd5-4e3f-46de-8c9d-469b496816d3&amp;at=AN_67v2vgmnRnUReCWDDCwrIVEFD:1727793849201</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1ySYl3sEFylupdOo3O-lO4ff6lUJVtM-q&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=e75a3b7c-ee4c-4550-b510-55af812beac5&amp;at=AN_67v0pMPGPYnfI1qi1_FyOGD1R:1727793857681</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1tZL5rR-ZeIJttsWYyz8_Sz5GmujetebL&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=09c0dce8-fd7a-41cf-8ef0-53cfac5dbff1&amp;at=AN_67v10MQMcSgXyaOURK-oCc641:1727793865552</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1vwoNDVHsoJ2i9bUYUv18nfumwBVvnE8U&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=e59e6ce8-8b03-4e25-943a-14d48baec665&amp;at=AN_67v2vBvr4k_A42rZ9noWSi_KN:1727793881049</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1bw603SJviRhJAD4VmEfEg2ZDDiwMhLoL&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=213983a2-399a-41e6-b259-8f6682ce2005&amp;at=AN_67v07yRNYtmAtaT3uIaFesahd:1727793891635</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1khWYlCPnD7Vf0v6Y_K0TsJ39UlW20UdA&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=02133a20-210d-40d8-af82-849dda15c500&amp;at=AN_67v0DrQDKTYPDQ0YIHRy-DesS:1727793899974</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1gxcSlNO9pMkkZMiHgAXB8CfG4kMDaBR3&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=49517128-e290-4414-ae8b-83a3ccc57027&amp;at=AN_67v38elmXKqBFIQw9ghzJIamv:1727793909205</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=13ecUVPuqBNhavP7MmDR399Bfa1oFO1mo&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=6ade43ee-13dc-48f4-8603-c7ee91e31a28&amp;at=AN_67v3gMpG_p2qTzJ_fAVWXlP5N:1727793922912</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1lVMOGchs1y8xhmYMlQU1AxHkCXmsHn_Z&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=38e90001-5a6b-46c9-af59-884936353192&amp;at=AN_67v2reTXHjuEzzYgKPASyn1cx:1727793930880</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=10754IBAsNO0pMSLL-pjYRZP1jFVitCZ5&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=04b50b5c-b127-4343-854d-e48a1f972081&amp;at=AN_67v2XHRgCFDCmt9VSP70SYF4G:1727793940011</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1BVhx3YBkrDxh9w2nw1tuU6iPAUJoIDDY&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=fe805a21-871a-4080-a335-807b329e1e1d&amp;at=AN_67v0urjQ-RZX0V6A71JJh63WP:1727793949180</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1Nn0fgVXD044N1jdBR9vrSm77EpA-oWSO&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=ae90a5a0-3ff0-4d2f-b603-83e4db1e6161&amp;at=AN_67v1e5kYNTorFsXQWt1kL1P4P:1727793957895</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1rDc0aLDcY8fUErsuYkXlAiNUSghm1pA7&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=0d211734-cbca-419a-b5a7-5ddb3bf60c59&amp;at=AN_67v2i0tKobmmJNZk-w9WI3-si:1727793966840</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1NyQk-V6o4eXBIfaqLh3Xx6wUH8ClCGhu&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=badc02cc-0f5e-4a17-9bf1-22b84065f3e5&amp;at=AN_67v35iuoZ8QylrSlQj9ylu6xe:1727793975063</t>
+  </si>
+  <si>
+    <t>https://drive.usercontent.google.com/download?id=1IK7FMUs-Pu_h_XZYc6VeV6LVpA63plLS&amp;export=download&amp;authuser=0&amp;confirm=t&amp;uuid=1bf0d0da-1f66-431b-a160-dc5108a400fe&amp;at=AN_67v3Xx0zfbdHzuhmYlNJWtso4:1727793979481</t>
+  </si>
+  <si>
+    <t>Special upload from CMAS</t>
+  </si>
+  <si>
+    <t>EQUATES_2003_inventory_onroad_01jun2021</t>
+  </si>
+  <si>
+    <t>EQUATES_2004_inventory_onroad_01jun2021</t>
+  </si>
+  <si>
+    <t>EQUATES_2005_inventory_onroad_23jun2021</t>
+  </si>
+  <si>
+    <t>EQUATES_2006_inventory_onroad_21may2021</t>
+  </si>
+  <si>
+    <t>EQUATES_2007_inventory_onroad_11may2021</t>
+  </si>
+  <si>
+    <t>EQUATES_2008_inventory_onroad_11may2021</t>
+  </si>
+  <si>
+    <t>EQUATES_2009_inventory_onroad_07may2021</t>
+  </si>
+  <si>
+    <t>EQUATES_2010_inventory_onroad_23jun2021</t>
+  </si>
+  <si>
+    <t>EQUATES_2011_inventory_onroad_20apr2021</t>
+  </si>
+  <si>
+    <t>EQUATES_2012_inventory_onroad_20apr2021</t>
+  </si>
+  <si>
+    <t>EQUATES_2014_inventory_onroad_01mar2021</t>
+  </si>
+  <si>
+    <t>EQUATES_2015_inventory_onroad_22feb2021</t>
+  </si>
+  <si>
+    <t>EQUATES_2016_inventory_onroad_18feb2021</t>
+  </si>
+  <si>
+    <t>EQUATES_2017_inventory_onroad_25jan2021</t>
+  </si>
+  <si>
+    <t>EQUATES_2018_inventory_onroad_31aug2021</t>
+  </si>
+  <si>
+    <t>EQUATES_2019_inventory_onroad_31aug2021</t>
+  </si>
+  <si>
+    <t>EQUATES_2002_inventory_onroad_01jun2021</t>
+  </si>
+  <si>
+    <t>EQUATES_INV_2002_version1.0</t>
+  </si>
+  <si>
+    <t>EQUATES_INV_2005_version1.0</t>
+  </si>
+  <si>
+    <t>EQUATES_INV_2008_version1.0</t>
+  </si>
+  <si>
+    <t>EQUATES_INV_2011_version1.0</t>
+  </si>
+  <si>
+    <t>EQUATES_INV_2014_version1.0</t>
+  </si>
+  <si>
+    <t>EQUATES_INV_2017_version1.0</t>
+  </si>
+  <si>
+    <t>EQUATES_INV_2019_version1.0</t>
+  </si>
+  <si>
+    <t>Special upload from CMAS. Contains N2O</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -908,6 +1040,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -942,7 +1087,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -959,6 +1104,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1411,10 +1560,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8EF959-18DF-BD43-B878-2D065289D72D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I167"/>
+  <dimension ref="A1:I185"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="123" workbookViewId="0">
-      <selection activeCell="C161" sqref="C161:C167"/>
+    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="123" workbookViewId="0">
+      <selection activeCell="G186" sqref="G186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1424,37 +1573,38 @@
     <col min="3" max="3" width="20.33203125" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.5" customWidth="1"/>
+    <col min="6" max="6" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5" customWidth="1"/>
     <col min="8" max="8" width="85.5" customWidth="1"/>
     <col min="9" max="9" width="115.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>223</v>
       </c>
     </row>
@@ -3127,48 +3277,52 @@
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>6</v>
-      </c>
-      <c r="B80">
+      <c r="A80" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" s="4">
         <v>2014</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D80" t="s">
-        <v>9</v>
-      </c>
-      <c r="F80" t="s">
+      <c r="D80" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="H80" t="s">
+      <c r="G80" s="4"/>
+      <c r="H80" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="I80" t="s">
+      <c r="I80" s="4" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>6</v>
-      </c>
-      <c r="B81">
+      <c r="A81" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" s="4">
         <v>2014</v>
       </c>
-      <c r="C81" t="s">
-        <v>47</v>
-      </c>
-      <c r="D81" t="s">
-        <v>9</v>
-      </c>
-      <c r="F81" t="s">
+      <c r="C81" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H81" t="s">
+      <c r="G81" s="4"/>
+      <c r="H81" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="I81" t="s">
+      <c r="I81" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3185,58 +3339,63 @@
       <c r="D82" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="E82" s="4"/>
       <c r="F82" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G82" s="1"/>
-      <c r="H82" s="8" t="s">
+      <c r="G82" s="5"/>
+      <c r="H82" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="I82" s="3" t="s">
+      <c r="I82" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>6</v>
-      </c>
-      <c r="B83">
+      <c r="A83" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" s="4">
         <v>2014</v>
       </c>
-      <c r="C83" t="s">
-        <v>47</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="C83" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D83" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="E83" s="4"/>
       <c r="F83" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G83" s="1"/>
-      <c r="H83" s="8" t="s">
+      <c r="G83" s="5"/>
+      <c r="H83" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="I83" s="3" t="s">
+      <c r="I83" s="11" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>6</v>
-      </c>
-      <c r="B84">
+      <c r="A84" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" s="4">
         <v>2014</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="G84" s="1" t="s">
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="H84" s="1"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="4"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
@@ -3251,111 +3410,117 @@
       <c r="D85" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F85" t="s">
+      <c r="E85" s="4"/>
+      <c r="F85" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="H85" t="s">
+      <c r="G85" s="4"/>
+      <c r="H85" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="I85" t="s">
+      <c r="I85" s="4" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+      <c r="A86" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="4">
         <v>2014</v>
       </c>
-      <c r="C86" t="s">
-        <v>47</v>
-      </c>
-      <c r="D86" t="s">
-        <v>9</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="C86" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G86" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H86" t="s">
+      <c r="H86" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="I86" t="s">
+      <c r="I86" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+      <c r="A87" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="4">
         <v>2014</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F87" t="s">
+      <c r="E87" s="4"/>
+      <c r="F87" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1" t="s">
+      <c r="G87" s="5"/>
+      <c r="H87" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I87" t="s">
+      <c r="I87" s="4" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+      <c r="A88" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="4">
         <v>2014</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F88" t="s">
+      <c r="E88" s="4"/>
+      <c r="F88" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1" t="s">
+      <c r="G88" s="5"/>
+      <c r="H88" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I88" t="s">
+      <c r="I88" s="4" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+      <c r="A89" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="4">
         <v>2014</v>
       </c>
-      <c r="C89" t="s">
-        <v>47</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="C89" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D89" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F89" t="s">
+      <c r="E89" s="4"/>
+      <c r="F89" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G89" s="1"/>
-      <c r="H89" s="1" t="s">
+      <c r="G89" s="5"/>
+      <c r="H89" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I89" t="s">
+      <c r="I89" s="4" t="s">
         <v>87</v>
       </c>
     </row>
@@ -4755,118 +4920,127 @@
       </c>
     </row>
     <row r="150" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
+      <c r="A150" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B150">
+      <c r="B150" s="4">
         <v>2014</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C150" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D150" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="F150" t="s">
+      <c r="E150" s="4"/>
+      <c r="F150" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="G150" s="1"/>
-      <c r="H150" s="1" t="s">
+      <c r="G150" s="5"/>
+      <c r="H150" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I150" t="s">
+      <c r="I150" s="4" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
+      <c r="A151" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B151">
+      <c r="B151" s="4">
         <v>2014</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C151" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D151" t="s">
-        <v>9</v>
-      </c>
-      <c r="F151" t="s">
+      <c r="D151" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E151" s="4"/>
+      <c r="F151" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="H151" s="1" t="s">
+      <c r="G151" s="4"/>
+      <c r="H151" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I151" t="s">
+      <c r="I151" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
+      <c r="A152" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B152">
+      <c r="B152" s="4">
         <v>2014</v>
       </c>
-      <c r="C152" t="s">
-        <v>47</v>
-      </c>
-      <c r="D152" t="s">
-        <v>9</v>
-      </c>
-      <c r="F152" t="s">
+      <c r="C152" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D152" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E152" s="4"/>
+      <c r="F152" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H152" s="1" t="s">
+      <c r="G152" s="4"/>
+      <c r="H152" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I152" t="s">
+      <c r="I152" s="4" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="153" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
+      <c r="A153" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B153">
+      <c r="B153" s="4">
         <v>2014</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C153" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D153" t="s">
-        <v>9</v>
-      </c>
-      <c r="F153" t="s">
+      <c r="D153" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E153" s="4"/>
+      <c r="F153" s="4" t="s">
         <v>247</v>
       </c>
+      <c r="G153" s="4"/>
       <c r="H153" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I153" s="3" t="s">
+      <c r="I153" s="11" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
+      <c r="A154" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B154">
+      <c r="B154" s="4">
         <v>2014</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C154" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D154" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F154" t="s">
+      <c r="E154" s="4"/>
+      <c r="F154" s="4" t="s">
         <v>247</v>
       </c>
+      <c r="G154" s="4"/>
       <c r="H154" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I154" s="3" t="s">
+      <c r="I154" s="11" t="s">
         <v>240</v>
       </c>
     </row>
@@ -4943,224 +5117,747 @@
       </c>
     </row>
     <row r="158" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
-        <v>6</v>
-      </c>
-      <c r="B158">
+      <c r="A158" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B158" s="4">
         <v>2014</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C158" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D158" t="s">
-        <v>9</v>
-      </c>
-      <c r="F158" t="s">
+      <c r="D158" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E158" s="4"/>
+      <c r="F158" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G158" t="s">
+      <c r="G158" s="4" t="s">
         <v>120</v>
       </c>
       <c r="H158" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I158" t="s">
+      <c r="I158" s="4" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
-        <v>6</v>
-      </c>
-      <c r="B159">
+      <c r="A159" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B159" s="4">
         <v>2014</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C159" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D159" t="s">
-        <v>9</v>
-      </c>
-      <c r="F159" t="s">
+      <c r="D159" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E159" s="4"/>
+      <c r="F159" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G159" t="s">
+      <c r="G159" s="4" t="s">
         <v>121</v>
       </c>
       <c r="H159" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I159" s="3" t="s">
+      <c r="I159" s="11" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
+      <c r="A160" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B160">
+      <c r="B160" s="4">
         <v>2014</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C160" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D160" t="s">
-        <v>9</v>
-      </c>
-      <c r="F160" t="s">
+      <c r="D160" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E160" s="4"/>
+      <c r="F160" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G160" t="s">
+      <c r="G160" s="4" t="s">
         <v>260</v>
       </c>
       <c r="H160" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I160" t="s">
+      <c r="I160" s="4" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
+      <c r="A161" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B161">
+      <c r="B161" s="4">
         <v>2002</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C161" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D161" t="s">
-        <v>9</v>
-      </c>
+      <c r="D161" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E161" s="4"/>
+      <c r="F161" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="G161" s="4"/>
       <c r="H161" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="I161" t="s">
+      <c r="I161" s="4" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
+      <c r="A162" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B162">
+      <c r="B162" s="4">
         <v>2005</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C162" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D162" t="s">
-        <v>9</v>
-      </c>
+      <c r="D162" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E162" s="4"/>
+      <c r="F162" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="G162" s="4"/>
       <c r="H162" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="I162" t="s">
+      <c r="I162" s="4" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
+      <c r="A163" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B163">
+      <c r="B163" s="4">
         <v>2008</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C163" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D163" t="s">
-        <v>9</v>
-      </c>
+      <c r="D163" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E163" s="4"/>
+      <c r="F163" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="G163" s="4"/>
       <c r="H163" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="I163" t="s">
+      <c r="I163" s="4" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
+      <c r="A164" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B164">
+      <c r="B164" s="4">
         <v>2011</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C164" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D164" t="s">
-        <v>9</v>
-      </c>
+      <c r="D164" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E164" s="4"/>
+      <c r="F164" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="G164" s="4"/>
       <c r="H164" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="I164" t="s">
+      <c r="I164" s="4" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A165" t="s">
+      <c r="A165" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B165">
+      <c r="B165" s="4">
         <v>2014</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C165" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D165" t="s">
-        <v>9</v>
-      </c>
+      <c r="D165" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E165" s="4"/>
+      <c r="F165" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="G165" s="4"/>
       <c r="H165" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="I165" t="s">
+      <c r="I165" s="4" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
+      <c r="A166" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B166">
+      <c r="B166" s="4">
         <v>2017</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C166" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D166" t="s">
-        <v>9</v>
-      </c>
+      <c r="D166" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E166" s="4"/>
+      <c r="F166" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="G166" s="4"/>
       <c r="H166" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="I166" t="s">
+      <c r="I166" s="4" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="167" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
+      <c r="A167" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B167">
+      <c r="B167" s="4">
         <v>2019</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C167" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D167" t="s">
-        <v>9</v>
-      </c>
-      <c r="G167" t="s">
+      <c r="D167" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E167" s="4"/>
+      <c r="F167" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="G167" s="4" t="s">
         <v>269</v>
       </c>
       <c r="H167" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="I167" t="s">
+      <c r="I167" s="4" t="s">
         <v>266</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A168" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B168" s="4">
+        <v>2002</v>
+      </c>
+      <c r="C168" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D168" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E168" s="4"/>
+      <c r="F168" t="s">
+        <v>308</v>
+      </c>
+      <c r="G168" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H168" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I168" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A169" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B169" s="4">
+        <v>2003</v>
+      </c>
+      <c r="C169" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D169" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E169" s="4"/>
+      <c r="F169" t="s">
+        <v>292</v>
+      </c>
+      <c r="G169" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H169" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I169" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A170" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B170" s="4">
+        <v>2004</v>
+      </c>
+      <c r="C170" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D170" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E170" s="4"/>
+      <c r="F170" t="s">
+        <v>293</v>
+      </c>
+      <c r="G170" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H170" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I170" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A171" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B171" s="4">
+        <v>2005</v>
+      </c>
+      <c r="C171" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D171" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E171" s="4"/>
+      <c r="F171" t="s">
+        <v>294</v>
+      </c>
+      <c r="G171" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H171" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I171" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A172" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B172" s="4">
+        <v>2006</v>
+      </c>
+      <c r="C172" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D172" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E172" s="4"/>
+      <c r="F172" t="s">
+        <v>295</v>
+      </c>
+      <c r="G172" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H172" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I172" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A173" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B173" s="4">
+        <v>2007</v>
+      </c>
+      <c r="C173" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D173" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E173" s="4"/>
+      <c r="F173" t="s">
+        <v>296</v>
+      </c>
+      <c r="G173" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H173" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I173" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A174" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B174" s="4">
+        <v>2008</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D174" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E174" s="4"/>
+      <c r="F174" t="s">
+        <v>297</v>
+      </c>
+      <c r="G174" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H174" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I174" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A175" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B175" s="4">
+        <v>2009</v>
+      </c>
+      <c r="C175" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D175" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E175" s="4"/>
+      <c r="F175" t="s">
+        <v>298</v>
+      </c>
+      <c r="G175" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H175" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I175" s="11" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A176" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B176" s="4">
+        <v>2010</v>
+      </c>
+      <c r="C176" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D176" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E176" s="4"/>
+      <c r="F176" t="s">
+        <v>299</v>
+      </c>
+      <c r="G176" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H176" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I176" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A177" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B177" s="4">
+        <v>2011</v>
+      </c>
+      <c r="C177" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D177" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E177" s="4"/>
+      <c r="F177" t="s">
+        <v>300</v>
+      </c>
+      <c r="G177" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H177" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I177" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A178" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B178" s="4">
+        <v>2012</v>
+      </c>
+      <c r="C178" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D178" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E178" s="4"/>
+      <c r="F178" t="s">
+        <v>301</v>
+      </c>
+      <c r="G178" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H178" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I178" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A179" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B179" s="4">
+        <v>2013</v>
+      </c>
+      <c r="C179" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D179" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E179" s="4"/>
+      <c r="F179" t="s">
+        <v>301</v>
+      </c>
+      <c r="G179" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H179" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I179" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A180" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B180" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C180" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D180" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E180" s="4"/>
+      <c r="F180" t="s">
+        <v>302</v>
+      </c>
+      <c r="G180" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H180" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I180" s="4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A181" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B181" s="4">
+        <v>2015</v>
+      </c>
+      <c r="C181" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D181" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E181" s="4"/>
+      <c r="F181" t="s">
+        <v>303</v>
+      </c>
+      <c r="G181" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H181" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I181" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A182" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B182" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C182" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D182" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E182" s="4"/>
+      <c r="F182" t="s">
+        <v>304</v>
+      </c>
+      <c r="G182" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H182" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I182" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A183" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B183" s="4">
+        <v>2017</v>
+      </c>
+      <c r="C183" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D183" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E183" s="4"/>
+      <c r="F183" t="s">
+        <v>305</v>
+      </c>
+      <c r="G183" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H183" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I183" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A184" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B184" s="4">
+        <v>2018</v>
+      </c>
+      <c r="C184" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D184" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E184" s="4"/>
+      <c r="F184" t="s">
+        <v>306</v>
+      </c>
+      <c r="G184" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="H184" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I184" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A185" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B185" s="4">
+        <v>2019</v>
+      </c>
+      <c r="C185" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D185" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E185" s="4"/>
+      <c r="F185" t="s">
+        <v>307</v>
+      </c>
+      <c r="G185" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="H185" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="I185" s="4" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -5212,6 +5909,7 @@
     <hyperlink ref="I153" r:id="rId12" xr:uid="{8AB8E0D9-B2E6-7A4B-B7FD-383AE4C17BF2}"/>
     <hyperlink ref="I154" r:id="rId13" xr:uid="{6702C906-A8EA-954F-8C17-7147195B6C53}"/>
     <hyperlink ref="I159" r:id="rId14" xr:uid="{AFDA6783-AFA0-A040-820E-4E25136EB298}"/>
+    <hyperlink ref="I175" r:id="rId15" xr:uid="{DD2C4424-579F-DF41-A73A-7ECFAD2F604F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update download links for 2022v1; re-run
no changes found
</commit_message>
<xml_diff>
--- a/_transportation/data-raw/epa/epa_downloads.xlsx
+++ b/_transportation/data-raw/epa/epa_downloads.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotenle/Documents/MetC_Locals/Interdivisional/ghg-cprg/_transportation/data-raw/epa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C680252D-41BD-4A46-BD4B-EA288431A6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACD3F1E-A53A-574A-BFB7-50FCD07CD69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17040" xr2:uid="{E3501ACA-8D46-AF4B-AC5D-95BB483C9130}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="notes" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$I$157</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$I$185</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="316">
   <si>
     <t>file_name</t>
   </si>
@@ -280,21 +280,12 @@
     <t>https://gaftp.epa.gov/air/nei/2020/data_summaries/2020nei_nonroad_byregion.zip</t>
   </si>
   <si>
-    <t>https://gaftp.epa.gov/Air/emismod/2021/2021emissions/nonroad_inventory_2021hb_24may2024.zip</t>
-  </si>
-  <si>
     <t>2021hb</t>
   </si>
   <si>
-    <t>https://gaftp.epa.gov/Air/emismod/2022/v1/2022emissions/onroad_emissions_SMOKE-MOVES_FF10_2022hc_17jul2024.zip</t>
-  </si>
-  <si>
     <t>2022hc</t>
   </si>
   <si>
-    <t>https://gaftp.epa.gov/Air/emismod/2022/v1/2022emissions/nonroad_inventory_2022hc_17jul2024.zip</t>
-  </si>
-  <si>
     <t>https://gaftp.epa.gov/Air/emismod/2021/2021emissions/onroad_emissions_SMOKE-MOVES_FF10_2021hb_26mar2024.zip</t>
   </si>
   <si>
@@ -463,9 +454,6 @@
     <t>https://gaftp.epa.gov/Air/emismod/2021/2021emissions/CDBs_2021_20240205.zip</t>
   </si>
   <si>
-    <t>https://gaftp.epa.gov/Air/emismod/2022/v1/2022emissions/onroad_activity_SMOKE-MOVES_FF10_2022hc_17jul2024.zip</t>
-  </si>
-  <si>
     <t>https://gaftp.epa.gov/Air/emismod/2022/v1/2022emissions/CDBs_2022_20240214.zip</t>
   </si>
   <si>
@@ -514,9 +502,6 @@
     <t>https://gaftp.epa.gov/Air/emismod/2021/info_2021hb_package_24may2024.txt</t>
   </si>
   <si>
-    <t>https://gaftp.epa.gov/Air/emismod/2022/v1/info_2022hc_package_prelim_version_10aug2024.txt</t>
-  </si>
-  <si>
     <t>https://gaftp.epa.gov/Air/emismod/2001/2001emis/readme_2001emis.txt</t>
   </si>
   <si>
@@ -992,6 +977,18 @@
   </si>
   <si>
     <t>Special upload from CMAS. Contains N2O</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/Air/emismod/2022/v1/2022emissions/2022hc_onroad_SMOKE-MOVES_MOVES4_emissions_FF10_23dec2024.zip</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/Air/emismod/2022/v1/2022emissions/2022hc_nonroad_inventory_20dec2024.zip</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/Air/emismod/2022/v1/info_2022v1_platform_package_24jan2025.txt</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/Air/emismod/2022/v1/2022emissions/2022hc_onroad_activity_20dec2024.zip</t>
   </si>
 </sst>
 </file>
@@ -1559,11 +1556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8EF959-18DF-BD43-B878-2D065289D72D}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="123" workbookViewId="0">
-      <selection activeCell="G186" sqref="G186"/>
+    <sheetView tabSelected="1" topLeftCell="F40" zoomScale="123" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1602,13 +1598,13 @@
         <v>1</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
@@ -1624,12 +1620,12 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1648,13 +1644,13 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -1670,12 +1666,12 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1683,22 +1679,22 @@
         <v>2001</v>
       </c>
       <c r="C5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="I5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1713,17 +1709,17 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1737,11 +1733,11 @@
         <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1755,11 +1751,11 @@
         <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1777,13 +1773,13 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1791,20 +1787,20 @@
         <v>2002</v>
       </c>
       <c r="C10" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D10" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="I10" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1821,13 +1817,13 @@
         <v>65</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -1835,22 +1831,22 @@
         <v>2002</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="H12" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I12" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1870,13 +1866,13 @@
         <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1884,17 +1880,17 @@
         <v>2003</v>
       </c>
       <c r="C14" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1908,11 +1904,11 @@
         <v>15</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1926,11 +1922,11 @@
         <v>9</v>
       </c>
       <c r="G16" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1938,17 +1934,17 @@
         <v>2004</v>
       </c>
       <c r="C17" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D17" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1962,11 +1958,11 @@
         <v>15</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1980,11 +1976,11 @@
         <v>9</v>
       </c>
       <c r="G19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1998,10 +1994,10 @@
         <v>9</v>
       </c>
       <c r="G20" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -2015,11 +2011,11 @@
         <v>15</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -2037,13 +2033,13 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="8" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="I22" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -2051,23 +2047,23 @@
         <v>2005</v>
       </c>
       <c r="C23" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D23" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F23" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="8" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="I23" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -2081,19 +2077,19 @@
         <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="G24" t="s">
         <v>55</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -2107,19 +2103,19 @@
         <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="G25" t="s">
         <v>56</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="I25" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>5</v>
       </c>
@@ -2127,22 +2123,22 @@
         <v>2005</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="H26" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="I26" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -2162,13 +2158,13 @@
         <v>22</v>
       </c>
       <c r="H27" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -2176,17 +2172,17 @@
         <v>2006</v>
       </c>
       <c r="C28" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -2200,11 +2196,11 @@
         <v>15</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -2218,10 +2214,10 @@
         <v>9</v>
       </c>
       <c r="G30" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -2229,17 +2225,17 @@
         <v>2007</v>
       </c>
       <c r="C31" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D31" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -2253,11 +2249,11 @@
         <v>15</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -2271,10 +2267,10 @@
         <v>9</v>
       </c>
       <c r="G33" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -2288,10 +2284,10 @@
         <v>9</v>
       </c>
       <c r="G34" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -2305,11 +2301,11 @@
         <v>15</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -2327,13 +2323,13 @@
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="I36" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -2341,20 +2337,20 @@
         <v>2008</v>
       </c>
       <c r="C37" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D37" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="I37" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -2371,13 +2367,13 @@
         <v>60</v>
       </c>
       <c r="H38" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="I38" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -2391,17 +2387,17 @@
         <v>15</v>
       </c>
       <c r="F39" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="I39" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -2409,23 +2405,23 @@
         <v>2008</v>
       </c>
       <c r="C40" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D40" t="s">
+        <v>167</v>
+      </c>
+      <c r="F40" t="s">
         <v>172</v>
-      </c>
-      <c r="F40" t="s">
-        <v>177</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="I40" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -2433,25 +2429,25 @@
         <v>2008</v>
       </c>
       <c r="C41" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D41" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F41" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G41" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="I41" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>72</v>
       </c>
@@ -2459,25 +2455,25 @@
         <v>2008</v>
       </c>
       <c r="C42" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" t="s">
+        <v>122</v>
+      </c>
+      <c r="F42" t="s">
+        <v>126</v>
+      </c>
+      <c r="G42" t="s">
+        <v>128</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I42" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D42" t="s">
-        <v>125</v>
-      </c>
-      <c r="F42" t="s">
-        <v>129</v>
-      </c>
-      <c r="G42" t="s">
-        <v>131</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -2485,25 +2481,25 @@
         <v>2008</v>
       </c>
       <c r="C43" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D43" t="s">
+        <v>122</v>
+      </c>
+      <c r="F43" t="s">
+        <v>126</v>
+      </c>
+      <c r="G43" t="s">
+        <v>129</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I43" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="F43" t="s">
-        <v>129</v>
-      </c>
-      <c r="G43" t="s">
-        <v>132</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>72</v>
       </c>
@@ -2520,13 +2516,13 @@
         <v>60</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="I44" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>5</v>
       </c>
@@ -2534,22 +2530,22 @@
         <v>2008</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F45" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="H45" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -2569,13 +2565,13 @@
         <v>27</v>
       </c>
       <c r="H46" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="I46" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -2583,17 +2579,17 @@
         <v>2009</v>
       </c>
       <c r="C47" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D47" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -2607,11 +2603,11 @@
         <v>15</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -2625,10 +2621,10 @@
         <v>9</v>
       </c>
       <c r="G49" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>6</v>
       </c>
@@ -2636,17 +2632,17 @@
         <v>2010</v>
       </c>
       <c r="C50" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D50" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>6</v>
       </c>
@@ -2660,11 +2656,11 @@
         <v>15</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -2678,10 +2674,10 @@
         <v>9</v>
       </c>
       <c r="G52" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -2698,13 +2694,13 @@
         <v>52</v>
       </c>
       <c r="H53" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I53" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -2718,19 +2714,19 @@
         <v>15</v>
       </c>
       <c r="F54" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>6</v>
       </c>
@@ -2744,19 +2740,19 @@
         <v>15</v>
       </c>
       <c r="F55" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="G55" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="I55" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="H55" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>6</v>
       </c>
@@ -2776,13 +2772,13 @@
         <v>56</v>
       </c>
       <c r="H56" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I56" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -2790,23 +2786,23 @@
         <v>2011</v>
       </c>
       <c r="C57" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D57" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F57" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I57" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -2826,13 +2822,13 @@
         <v>55</v>
       </c>
       <c r="H58" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I58" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>72</v>
       </c>
@@ -2846,17 +2842,17 @@
         <v>15</v>
       </c>
       <c r="F59" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="I59" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -2870,17 +2866,17 @@
         <v>15</v>
       </c>
       <c r="F60" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="I60" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>72</v>
       </c>
@@ -2888,23 +2884,23 @@
         <v>2011</v>
       </c>
       <c r="C61" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D61" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F61" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="I61" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>72</v>
       </c>
@@ -2912,25 +2908,25 @@
         <v>2011</v>
       </c>
       <c r="C62" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D62" t="s">
         <v>9</v>
       </c>
       <c r="F62" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G62" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="I62" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>72</v>
       </c>
@@ -2938,25 +2934,25 @@
         <v>2011</v>
       </c>
       <c r="C63" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D63" t="s">
         <v>9</v>
       </c>
       <c r="F63" t="s">
+        <v>115</v>
+      </c>
+      <c r="G63" t="s">
         <v>118</v>
       </c>
-      <c r="G63" t="s">
-        <v>121</v>
-      </c>
       <c r="H63" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="I63" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>5</v>
       </c>
@@ -2964,22 +2960,22 @@
         <v>2011</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F64" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="H64" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="I64" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>72</v>
       </c>
@@ -2993,16 +2989,16 @@
         <v>9</v>
       </c>
       <c r="F65" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="I65" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -3022,13 +3018,13 @@
         <v>28</v>
       </c>
       <c r="H66" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="I66" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -3042,10 +3038,10 @@
         <v>9</v>
       </c>
       <c r="G67" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -3059,11 +3055,11 @@
         <v>15</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -3071,17 +3067,17 @@
         <v>2012</v>
       </c>
       <c r="C69" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D69" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -3095,11 +3091,11 @@
         <v>15</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>6</v>
       </c>
@@ -3113,10 +3109,10 @@
         <v>9</v>
       </c>
       <c r="G71" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>6</v>
       </c>
@@ -3130,10 +3126,10 @@
         <v>9</v>
       </c>
       <c r="G72" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>6</v>
       </c>
@@ -3149,12 +3145,12 @@
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
       <c r="G73" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H73" s="5"/>
       <c r="I73" s="4"/>
     </row>
-    <row r="74" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -3168,11 +3164,11 @@
         <v>15</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>6</v>
       </c>
@@ -3186,10 +3182,10 @@
         <v>9</v>
       </c>
       <c r="G75" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>6</v>
       </c>
@@ -3197,17 +3193,17 @@
         <v>2013</v>
       </c>
       <c r="C76" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D76" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>72</v>
       </c>
@@ -3215,25 +3211,25 @@
         <v>2011</v>
       </c>
       <c r="C77" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D77" t="s">
         <v>9</v>
       </c>
       <c r="F77" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="G77" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I77" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>72</v>
       </c>
@@ -3241,22 +3237,22 @@
         <v>2011</v>
       </c>
       <c r="C78" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D78" t="s">
         <v>9</v>
       </c>
       <c r="G78" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I78" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>72</v>
       </c>
@@ -3264,16 +3260,16 @@
         <v>2011</v>
       </c>
       <c r="C79" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D79" t="s">
         <v>15</v>
       </c>
       <c r="F79" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
@@ -3291,14 +3287,14 @@
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G80" s="4"/>
       <c r="H80" s="4" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
@@ -3320,7 +3316,7 @@
       </c>
       <c r="G81" s="4"/>
       <c r="H81" s="4" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I81" s="4" t="s">
         <v>39</v>
@@ -3341,14 +3337,14 @@
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G82" s="5"/>
       <c r="H82" s="10" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I82" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3366,14 +3362,14 @@
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G83" s="5"/>
       <c r="H83" s="10" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I83" s="11" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3384,15 +3380,15 @@
         <v>2014</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
       <c r="G84" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H84" s="5"/>
       <c r="I84" s="4"/>
@@ -3405,21 +3401,21 @@
         <v>2014</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="G85" s="4"/>
       <c r="H85" s="4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
@@ -3443,7 +3439,7 @@
         <v>29</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="I86" s="4" t="s">
         <v>33</v>
@@ -3457,21 +3453,21 @@
         <v>2014</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G87" s="5"/>
       <c r="H87" s="5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3482,21 +3478,21 @@
         <v>2014</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G88" s="5"/>
       <c r="H88" s="5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3514,17 +3510,17 @@
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G89" s="5"/>
       <c r="H89" s="5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>6</v>
       </c>
@@ -3541,13 +3537,13 @@
         <v>37</v>
       </c>
       <c r="H90" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I90" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>6</v>
       </c>
@@ -3564,16 +3560,16 @@
         <v>37</v>
       </c>
       <c r="G91" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H91" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I91" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -3590,13 +3586,13 @@
         <v>37</v>
       </c>
       <c r="H92" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I92" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -3614,13 +3610,13 @@
       </c>
       <c r="G93" s="1"/>
       <c r="H93" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I93" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>6</v>
       </c>
@@ -3634,12 +3630,12 @@
         <v>15</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H94" s="1"/>
       <c r="I94" s="3"/>
     </row>
-    <row r="95" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -3647,20 +3643,20 @@
         <v>2015</v>
       </c>
       <c r="C95" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D95" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G95" s="1"/>
       <c r="H95" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="I95" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -3674,16 +3670,16 @@
         <v>9</v>
       </c>
       <c r="F96" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H96" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="I96" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>6</v>
       </c>
@@ -3700,13 +3696,13 @@
         <v>43</v>
       </c>
       <c r="H97" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="I97" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>6</v>
       </c>
@@ -3714,23 +3710,23 @@
         <v>2016</v>
       </c>
       <c r="C98" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D98" t="s">
         <v>15</v>
       </c>
       <c r="F98" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G98" s="1"/>
       <c r="H98" s="8" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="I98" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>6</v>
       </c>
@@ -3744,17 +3740,17 @@
         <v>15</v>
       </c>
       <c r="F99" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G99" s="1"/>
       <c r="H99" s="8" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="I99" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>6</v>
       </c>
@@ -3762,20 +3758,20 @@
         <v>2016</v>
       </c>
       <c r="C100" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D100" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G100" s="1"/>
       <c r="H100" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="I100" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>6</v>
       </c>
@@ -3792,13 +3788,13 @@
         <v>13</v>
       </c>
       <c r="H101" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="I101" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>6</v>
       </c>
@@ -3815,13 +3811,13 @@
         <v>13</v>
       </c>
       <c r="H102" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="I102" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>6</v>
       </c>
@@ -3835,11 +3831,11 @@
         <v>15</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H103" s="1"/>
     </row>
-    <row r="104" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>6</v>
       </c>
@@ -3857,13 +3853,13 @@
       </c>
       <c r="G104" s="1"/>
       <c r="H104" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="I104" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -3871,23 +3867,23 @@
         <v>2017</v>
       </c>
       <c r="C105" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D105" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F105" t="s">
         <v>13</v>
       </c>
       <c r="G105" s="1"/>
       <c r="H105" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="I105" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>5</v>
       </c>
@@ -3895,22 +3891,22 @@
         <v>2017</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F106" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="H106" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="I106" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>5</v>
       </c>
@@ -3927,13 +3923,13 @@
         <v>26</v>
       </c>
       <c r="H107" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="I107" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>5</v>
       </c>
@@ -3953,13 +3949,13 @@
         <v>30</v>
       </c>
       <c r="H108" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="I108" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>72</v>
       </c>
@@ -3967,23 +3963,23 @@
         <v>2017</v>
       </c>
       <c r="C109" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D109" t="s">
         <v>15</v>
       </c>
       <c r="F109" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G109" s="1"/>
       <c r="H109" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I109" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>72</v>
       </c>
@@ -4000,16 +3996,16 @@
         <v>76</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I110" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>72</v>
       </c>
@@ -4017,23 +4013,23 @@
         <v>2017</v>
       </c>
       <c r="C111" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D111" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F111" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="G111" s="1"/>
       <c r="H111" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I111" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>72</v>
       </c>
@@ -4047,16 +4043,16 @@
         <v>9</v>
       </c>
       <c r="F112" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I112" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>72</v>
       </c>
@@ -4073,16 +4069,16 @@
         <v>76</v>
       </c>
       <c r="G113" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I113" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -4096,16 +4092,16 @@
         <v>9</v>
       </c>
       <c r="F114" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H114" s="8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I114" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>6</v>
       </c>
@@ -4119,16 +4115,16 @@
         <v>9</v>
       </c>
       <c r="F115" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="H115" s="8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I115" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>6</v>
       </c>
@@ -4136,20 +4132,20 @@
         <v>2018</v>
       </c>
       <c r="C116" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D116" t="s">
         <v>15</v>
       </c>
       <c r="G116" s="1"/>
       <c r="H116" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I116" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>6</v>
       </c>
@@ -4167,13 +4163,13 @@
       </c>
       <c r="G117" s="1"/>
       <c r="H117" s="8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I117" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>6</v>
       </c>
@@ -4181,23 +4177,23 @@
         <v>2018</v>
       </c>
       <c r="C118" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D118" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F118" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G118" s="1"/>
       <c r="H118" s="8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I118" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>6</v>
       </c>
@@ -4205,23 +4201,23 @@
         <v>2018</v>
       </c>
       <c r="C119" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D119" t="s">
+        <v>144</v>
+      </c>
+      <c r="F119" t="s">
         <v>148</v>
-      </c>
-      <c r="F119" t="s">
-        <v>152</v>
       </c>
       <c r="G119" s="1"/>
       <c r="H119" s="8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I119" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>6</v>
       </c>
@@ -4235,16 +4231,16 @@
         <v>9</v>
       </c>
       <c r="F120" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H120" s="8" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="I120" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>6</v>
       </c>
@@ -4261,13 +4257,13 @@
         <v>41</v>
       </c>
       <c r="H121" s="8" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="I121" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>6</v>
       </c>
@@ -4275,20 +4271,20 @@
         <v>2019</v>
       </c>
       <c r="C122" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D122" t="s">
         <v>15</v>
       </c>
       <c r="G122" s="1"/>
       <c r="H122" s="8" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="I122" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>6</v>
       </c>
@@ -4296,23 +4292,23 @@
         <v>2019</v>
       </c>
       <c r="C123" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D123" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F123" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G123" s="1"/>
       <c r="H123" s="8" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="I123" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>6</v>
       </c>
@@ -4326,17 +4322,17 @@
         <v>15</v>
       </c>
       <c r="F124" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G124" s="1"/>
       <c r="H124" s="8" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="I124" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>6</v>
       </c>
@@ -4350,16 +4346,16 @@
         <v>9</v>
       </c>
       <c r="F125" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H125" s="8" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="I125" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>6</v>
       </c>
@@ -4376,13 +4372,13 @@
         <v>36</v>
       </c>
       <c r="H126" s="8" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="I126" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>6</v>
       </c>
@@ -4390,17 +4386,17 @@
         <v>2020</v>
       </c>
       <c r="C127" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D127" t="s">
         <v>15</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H127" s="8"/>
     </row>
-    <row r="128" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>6</v>
       </c>
@@ -4418,13 +4414,13 @@
       </c>
       <c r="G128" s="1"/>
       <c r="H128" s="8" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="I128" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>6</v>
       </c>
@@ -4432,23 +4428,23 @@
         <v>2020</v>
       </c>
       <c r="C129" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D129" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F129" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G129" s="1"/>
       <c r="H129" s="8" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="I129" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>72</v>
       </c>
@@ -4456,23 +4452,23 @@
         <v>2020</v>
       </c>
       <c r="C130" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D130" t="s">
         <v>15</v>
       </c>
       <c r="F130" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G130" s="1"/>
       <c r="H130" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="I130" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>72</v>
       </c>
@@ -4490,13 +4486,13 @@
       </c>
       <c r="G131" s="1"/>
       <c r="H131" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="I131" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>72</v>
       </c>
@@ -4504,20 +4500,20 @@
         <v>2020</v>
       </c>
       <c r="C132" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D132" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G132" s="1"/>
       <c r="H132" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="I132" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>72</v>
       </c>
@@ -4531,16 +4527,16 @@
         <v>9</v>
       </c>
       <c r="F133" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="I133" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>72</v>
       </c>
@@ -4548,22 +4544,22 @@
         <v>2020</v>
       </c>
       <c r="C134" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D134" t="s">
         <v>9</v>
       </c>
       <c r="F134" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H134" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="I134" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>72</v>
       </c>
@@ -4571,22 +4567,22 @@
         <v>2020</v>
       </c>
       <c r="C135" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D135" t="s">
         <v>15</v>
       </c>
       <c r="F135" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="I135" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>72</v>
       </c>
@@ -4603,13 +4599,13 @@
         <v>77</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="I136" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>6</v>
       </c>
@@ -4623,16 +4619,16 @@
         <v>9</v>
       </c>
       <c r="F137" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="I137" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>6</v>
       </c>
@@ -4647,17 +4643,17 @@
       </c>
       <c r="E138" s="4"/>
       <c r="F138" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G138" s="4"/>
       <c r="H138" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="I138" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>6</v>
       </c>
@@ -4665,20 +4661,20 @@
         <v>2021</v>
       </c>
       <c r="C139" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D139" t="s">
         <v>15</v>
       </c>
       <c r="G139" s="1"/>
       <c r="H139" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="I139" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>6</v>
       </c>
@@ -4692,17 +4688,17 @@
         <v>15</v>
       </c>
       <c r="F140" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G140" s="1"/>
       <c r="H140" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="I140" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>6</v>
       </c>
@@ -4710,23 +4706,23 @@
         <v>2021</v>
       </c>
       <c r="C141" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D141" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F141" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G141" s="1"/>
       <c r="H141" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="I141" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>6</v>
       </c>
@@ -4740,16 +4736,16 @@
         <v>9</v>
       </c>
       <c r="F142" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H142" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="I142" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>6</v>
       </c>
@@ -4764,17 +4760,17 @@
       </c>
       <c r="E143" s="4"/>
       <c r="F143" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G143" s="4"/>
       <c r="H143" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="I143" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>6</v>
       </c>
@@ -4782,20 +4778,20 @@
         <v>2022</v>
       </c>
       <c r="C144" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D144" t="s">
         <v>15</v>
       </c>
       <c r="G144" s="1"/>
       <c r="H144" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="I144" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>6</v>
       </c>
@@ -4810,17 +4806,17 @@
       </c>
       <c r="E145" s="4"/>
       <c r="F145" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G145" s="5"/>
       <c r="H145" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="I145" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+      <c r="I145" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>6</v>
       </c>
@@ -4828,23 +4824,23 @@
         <v>2022</v>
       </c>
       <c r="C146" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D146" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F146" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G146" s="1"/>
       <c r="H146" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="I146" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+      <c r="I146" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>72</v>
       </c>
@@ -4852,25 +4848,25 @@
         <v>2017</v>
       </c>
       <c r="C147" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D147" t="s">
         <v>9</v>
       </c>
       <c r="F147" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G147" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H147" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I147" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>72</v>
       </c>
@@ -4878,25 +4874,25 @@
         <v>2017</v>
       </c>
       <c r="C148" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D148" t="s">
         <v>9</v>
       </c>
       <c r="F148" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G148" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H148" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I148" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>72</v>
       </c>
@@ -4910,13 +4906,13 @@
         <v>15</v>
       </c>
       <c r="F149" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H149" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I149" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="150" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4927,21 +4923,21 @@
         <v>2014</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E150" s="4"/>
       <c r="F150" s="4" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G150" s="5"/>
       <c r="H150" s="5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I150" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4959,14 +4955,14 @@
       </c>
       <c r="E151" s="4"/>
       <c r="F151" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G151" s="4"/>
       <c r="H151" s="5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I151" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4984,14 +4980,14 @@
       </c>
       <c r="E152" s="4"/>
       <c r="F152" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G152" s="4"/>
       <c r="H152" s="5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I152" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="153" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5002,21 +4998,21 @@
         <v>2014</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D153" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E153" s="4"/>
       <c r="F153" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="G153" s="4"/>
       <c r="H153" s="5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I153" s="11" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5027,24 +5023,24 @@
         <v>2014</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D154" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E154" s="4"/>
       <c r="F154" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="G154" s="4"/>
       <c r="H154" s="5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I154" s="11" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>72</v>
       </c>
@@ -5052,7 +5048,7 @@
         <v>2008</v>
       </c>
       <c r="C155" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D155" t="s">
         <v>9</v>
@@ -5061,13 +5057,13 @@
         <v>60</v>
       </c>
       <c r="H155" s="5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="I155" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="156" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>72</v>
       </c>
@@ -5075,7 +5071,7 @@
         <v>2008</v>
       </c>
       <c r="C156" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D156" t="s">
         <v>15</v>
@@ -5084,13 +5080,13 @@
         <v>60</v>
       </c>
       <c r="H156" s="5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="I156" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>72</v>
       </c>
@@ -5104,16 +5100,16 @@
         <v>9</v>
       </c>
       <c r="F157" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G157" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H157" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I157" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="158" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5124,23 +5120,23 @@
         <v>2014</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D158" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E158" s="4"/>
       <c r="F158" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G158" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H158" s="5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I158" s="4" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5151,23 +5147,23 @@
         <v>2014</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D159" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E159" s="4"/>
       <c r="F159" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G159" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H159" s="5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I159" s="11" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5178,23 +5174,23 @@
         <v>2014</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D160" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E160" s="4"/>
       <c r="F160" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G160" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="H160" s="5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I160" s="4" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5205,21 +5201,21 @@
         <v>2002</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D161" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E161" s="4"/>
       <c r="F161" s="4" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="G161" s="4"/>
       <c r="H161" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I161" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5230,21 +5226,21 @@
         <v>2005</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D162" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E162" s="4"/>
       <c r="F162" s="4" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="G162" s="4"/>
       <c r="H162" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I162" s="4" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5255,21 +5251,21 @@
         <v>2008</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D163" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E163" s="4"/>
       <c r="F163" s="4" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G163" s="4"/>
       <c r="H163" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I163" s="4" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5280,21 +5276,21 @@
         <v>2011</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D164" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E164" s="4"/>
       <c r="F164" s="4" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="G164" s="4"/>
       <c r="H164" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I164" s="4" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5305,21 +5301,21 @@
         <v>2014</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D165" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E165" s="4"/>
       <c r="F165" s="4" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="G165" s="4"/>
       <c r="H165" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I165" s="4" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5330,21 +5326,21 @@
         <v>2017</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D166" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E166" s="4"/>
       <c r="F166" s="4" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G166" s="4"/>
       <c r="H166" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I166" s="4" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="167" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5355,23 +5351,23 @@
         <v>2019</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D167" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E167" s="4"/>
       <c r="F167" s="4" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="G167" s="4" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="H167" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I167" s="4" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="168" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5382,23 +5378,23 @@
         <v>2002</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D168" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E168" s="4"/>
       <c r="F168" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="G168" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H168" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="I168" s="4" t="s">
         <v>268</v>
-      </c>
-      <c r="I168" s="4" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5409,23 +5405,23 @@
         <v>2003</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D169" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E169" s="4"/>
       <c r="F169" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="G169" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H169" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I169" s="4" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="170" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5436,23 +5432,23 @@
         <v>2004</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D170" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E170" s="4"/>
       <c r="F170" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="G170" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H170" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I170" s="4" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5463,23 +5459,23 @@
         <v>2005</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D171" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E171" s="4"/>
       <c r="F171" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="G171" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H171" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I171" s="4" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="172" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5490,23 +5486,23 @@
         <v>2006</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D172" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E172" s="4"/>
       <c r="F172" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="G172" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H172" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I172" s="4" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5517,23 +5513,23 @@
         <v>2007</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D173" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E173" s="4"/>
       <c r="F173" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G173" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H173" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I173" s="4" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="174" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5544,23 +5540,23 @@
         <v>2008</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D174" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E174" s="4"/>
       <c r="F174" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="G174" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H174" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I174" s="4" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="175" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5571,23 +5567,23 @@
         <v>2009</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D175" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E175" s="4"/>
       <c r="F175" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="G175" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H175" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I175" s="11" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="176" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5598,23 +5594,23 @@
         <v>2010</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D176" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E176" s="4"/>
       <c r="F176" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="G176" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H176" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I176" s="4" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="177" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5625,23 +5621,23 @@
         <v>2011</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D177" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E177" s="4"/>
       <c r="F177" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="G177" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H177" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I177" s="4" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="178" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5652,23 +5648,23 @@
         <v>2012</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D178" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E178" s="4"/>
       <c r="F178" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G178" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H178" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I178" s="4" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="179" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5679,23 +5675,23 @@
         <v>2013</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D179" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E179" s="4"/>
       <c r="F179" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="G179" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H179" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I179" s="4" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="180" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5706,23 +5702,23 @@
         <v>2014</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D180" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E180" s="4"/>
       <c r="F180" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="G180" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H180" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I180" s="4" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="181" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5733,23 +5729,23 @@
         <v>2015</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D181" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E181" s="4"/>
       <c r="F181" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="G181" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H181" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I181" s="4" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5760,23 +5756,23 @@
         <v>2016</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D182" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E182" s="4"/>
       <c r="F182" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="G182" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H182" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I182" s="4" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="183" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5787,23 +5783,23 @@
         <v>2017</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D183" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E183" s="4"/>
       <c r="F183" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="G183" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H183" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I183" s="4" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="184" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5814,23 +5810,23 @@
         <v>2018</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D184" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E184" s="4"/>
       <c r="F184" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G184" s="4" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="H184" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I184" s="4" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5841,32 +5837,27 @@
         <v>2019</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D185" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E185" s="4"/>
       <c r="F185" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="G185" s="4" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="H185" s="5" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I185" s="4" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I157" xr:uid="{EB8EF959-18DF-BD43-B878-2D065289D72D}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="2014"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A1:I185" xr:uid="{EB8EF959-18DF-BD43-B878-2D065289D72D}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A53:I154">
       <sortCondition ref="B1:B156"/>
     </sortState>
@@ -5910,6 +5901,7 @@
     <hyperlink ref="I154" r:id="rId13" xr:uid="{6702C906-A8EA-954F-8C17-7147195B6C53}"/>
     <hyperlink ref="I159" r:id="rId14" xr:uid="{AFDA6783-AFA0-A040-820E-4E25136EB298}"/>
     <hyperlink ref="I175" r:id="rId15" xr:uid="{DD2C4424-579F-DF41-A73A-7ECFAD2F604F}"/>
+    <hyperlink ref="I146" r:id="rId16" xr:uid="{78D2C5DD-3713-844A-92AC-6998C8206DEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5934,7 +5926,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -5942,7 +5934,7 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -5950,7 +5942,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -5958,15 +5950,15 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B5" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -5986,37 +5978,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
render epa download documentation
</commit_message>
<xml_diff>
--- a/_transportation/data-raw/epa/epa_downloads.xlsx
+++ b/_transportation/data-raw/epa/epa_downloads.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rotenle/Documents/MetC_Locals/Interdivisional/ghg-cprg/_transportation/data-raw/epa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C502CDB-521C-0E43-98DD-20FC01B47F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3051464F-6DC6-D840-9EAE-A4269DC3BFED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="900" windowWidth="30720" windowHeight="17040" xr2:uid="{E3501ACA-8D46-AF4B-AC5D-95BB483C9130}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="notes" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$I$187</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">index!$A$1:$I$189</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="323">
   <si>
     <t>file_name</t>
   </si>
@@ -292,9 +292,6 @@
     <t>2022hc</t>
   </si>
   <si>
-    <t>https://gaftp.epa.gov/Air/emismod/2022/v1/2022emissions/nonroad_inventory_2022hc_17jul2024.zip</t>
-  </si>
-  <si>
     <t>https://gaftp.epa.gov/Air/emismod/2021/2021emissions/onroad_emissions_SMOKE-MOVES_FF10_2021hb_26mar2024.zip</t>
   </si>
   <si>
@@ -997,10 +994,22 @@
     <t>2022hd</t>
   </si>
   <si>
-    <t>https://gaftp.epa.gov/Air/emismod/2022/v2/2022emissions/draft/2022hd_onroad_SMOKE-MOVES_inventory_19jun2025.zip</t>
-  </si>
-  <si>
     <t>https://gaftp.epa.gov/Air/emismod/2022/v2/reports/2022v2_emissions_docn.pdf</t>
+  </si>
+  <si>
+    <t>_transportation/data-raw/epa/air_emissions_modeling/2022v2</t>
+  </si>
+  <si>
+    <t>2022he</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/Air/emismod/2022/v2/2022emissions/2022he_onroad_SMOKE-MOVES_inventory_19jun2025.zip</t>
+  </si>
+  <si>
+    <t>https://gaftp.epa.gov/Air/emismod/2022/v2/2022emissions/2022he_nonroad_inventory_26aug2025.zip</t>
+  </si>
+  <si>
+    <t>https://epa-2022-modeling-platform.s3.amazonaws.com/emis/2022v2/2022he_cb6_22m/moves_eftables/st27_2022he_eftables_caps.zip</t>
   </si>
 </sst>
 </file>
@@ -1568,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8EF959-18DF-BD43-B878-2D065289D72D}">
-  <dimension ref="A1:I187"/>
+  <dimension ref="A1:I189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="123" workbookViewId="0">
-      <selection activeCell="E147" sqref="E147"/>
+    <sheetView tabSelected="1" topLeftCell="H135" zoomScale="123" workbookViewId="0">
+      <selection activeCell="I150" sqref="I150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1610,10 +1619,10 @@
         <v>1</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1632,7 +1641,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="6"/>
@@ -1656,7 +1665,7 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>66</v>
@@ -1678,7 +1687,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -1691,19 +1700,19 @@
         <v>2001</v>
       </c>
       <c r="C5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1721,11 +1730,11 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>68</v>
@@ -1745,7 +1754,7 @@
         <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -1763,7 +1772,7 @@
         <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -1785,7 +1794,7 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>64</v>
@@ -1799,17 +1808,17 @@
         <v>2002</v>
       </c>
       <c r="C10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1829,7 +1838,7 @@
         <v>65</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>69</v>
@@ -1843,19 +1852,19 @@
         <v>2002</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1878,7 +1887,7 @@
         <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>17</v>
@@ -1892,13 +1901,13 @@
         <v>2003</v>
       </c>
       <c r="C14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -1916,7 +1925,7 @@
         <v>15</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -1934,7 +1943,7 @@
         <v>9</v>
       </c>
       <c r="G16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I16" s="3"/>
     </row>
@@ -1946,13 +1955,13 @@
         <v>2004</v>
       </c>
       <c r="C17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -1970,7 +1979,7 @@
         <v>15</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -1988,7 +1997,7 @@
         <v>9</v>
       </c>
       <c r="G19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I19" s="3"/>
     </row>
@@ -2006,7 +2015,7 @@
         <v>9</v>
       </c>
       <c r="G20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2023,7 +2032,7 @@
         <v>15</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H21" s="1"/>
     </row>
@@ -2045,7 +2054,7 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I22" t="s">
         <v>62</v>
@@ -2059,20 +2068,20 @@
         <v>2005</v>
       </c>
       <c r="C23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2089,13 +2098,13 @@
         <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G24" t="s">
         <v>55</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>70</v>
@@ -2115,13 +2124,13 @@
         <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G25" t="s">
         <v>56</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I25" t="s">
         <v>71</v>
@@ -2135,19 +2144,19 @@
         <v>2005</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H26" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -2170,7 +2179,7 @@
         <v>22</v>
       </c>
       <c r="H27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>21</v>
@@ -2184,13 +2193,13 @@
         <v>2006</v>
       </c>
       <c r="C28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H28" s="1"/>
     </row>
@@ -2208,7 +2217,7 @@
         <v>15</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H29" s="1"/>
     </row>
@@ -2226,7 +2235,7 @@
         <v>9</v>
       </c>
       <c r="G30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2237,13 +2246,13 @@
         <v>2007</v>
       </c>
       <c r="C31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H31" s="1"/>
     </row>
@@ -2261,7 +2270,7 @@
         <v>15</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H32" s="1"/>
     </row>
@@ -2279,7 +2288,7 @@
         <v>9</v>
       </c>
       <c r="G33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -2296,7 +2305,7 @@
         <v>9</v>
       </c>
       <c r="G34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2313,7 +2322,7 @@
         <v>15</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H35" s="1"/>
     </row>
@@ -2335,7 +2344,7 @@
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I36" t="s">
         <v>61</v>
@@ -2349,17 +2358,17 @@
         <v>2008</v>
       </c>
       <c r="C37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I37" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -2379,7 +2388,7 @@
         <v>60</v>
       </c>
       <c r="H38" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I38" t="s">
         <v>59</v>
@@ -2399,14 +2408,14 @@
         <v>15</v>
       </c>
       <c r="F39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2417,20 +2426,20 @@
         <v>2008</v>
       </c>
       <c r="C40" t="s">
+        <v>170</v>
+      </c>
+      <c r="D40" t="s">
         <v>171</v>
       </c>
-      <c r="D40" t="s">
-        <v>172</v>
-      </c>
       <c r="F40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2441,22 +2450,22 @@
         <v>2008</v>
       </c>
       <c r="C41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D41" t="s">
         <v>124</v>
       </c>
-      <c r="D41" t="s">
+      <c r="F41" t="s">
+        <v>128</v>
+      </c>
+      <c r="G41" t="s">
+        <v>129</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I41" t="s">
         <v>125</v>
-      </c>
-      <c r="F41" t="s">
-        <v>129</v>
-      </c>
-      <c r="G41" t="s">
-        <v>130</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="I41" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2467,22 +2476,22 @@
         <v>2008</v>
       </c>
       <c r="C42" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" t="s">
         <v>124</v>
       </c>
-      <c r="D42" t="s">
-        <v>125</v>
-      </c>
       <c r="F42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G42" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2493,22 +2502,22 @@
         <v>2008</v>
       </c>
       <c r="C43" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" t="s">
         <v>124</v>
       </c>
-      <c r="D43" t="s">
-        <v>125</v>
-      </c>
       <c r="F43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G43" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2528,10 +2537,10 @@
         <v>60</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -2542,19 +2551,19 @@
         <v>2008</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F45" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H45" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -2577,7 +2586,7 @@
         <v>27</v>
       </c>
       <c r="H46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I46" t="s">
         <v>31</v>
@@ -2591,13 +2600,13 @@
         <v>2009</v>
       </c>
       <c r="C47" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H47" s="1"/>
     </row>
@@ -2615,7 +2624,7 @@
         <v>15</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H48" s="1"/>
     </row>
@@ -2633,7 +2642,7 @@
         <v>9</v>
       </c>
       <c r="G49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2644,13 +2653,13 @@
         <v>2010</v>
       </c>
       <c r="C50" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H50" s="1"/>
     </row>
@@ -2668,7 +2677,7 @@
         <v>15</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H51" s="1"/>
     </row>
@@ -2686,7 +2695,7 @@
         <v>9</v>
       </c>
       <c r="G52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -2706,7 +2715,7 @@
         <v>52</v>
       </c>
       <c r="H53" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I53" t="s">
         <v>53</v>
@@ -2726,16 +2735,16 @@
         <v>15</v>
       </c>
       <c r="F54" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2752,16 +2761,16 @@
         <v>15</v>
       </c>
       <c r="F55" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
@@ -2784,7 +2793,7 @@
         <v>56</v>
       </c>
       <c r="H56" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I56" t="s">
         <v>57</v>
@@ -2798,20 +2807,20 @@
         <v>2011</v>
       </c>
       <c r="C57" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F57" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I57" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -2834,7 +2843,7 @@
         <v>55</v>
       </c>
       <c r="H58" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I58" t="s">
         <v>54</v>
@@ -2854,14 +2863,14 @@
         <v>15</v>
       </c>
       <c r="F59" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I59" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2878,14 +2887,14 @@
         <v>15</v>
       </c>
       <c r="F60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2896,20 +2905,20 @@
         <v>2011</v>
       </c>
       <c r="C61" t="s">
+        <v>170</v>
+      </c>
+      <c r="D61" t="s">
         <v>171</v>
       </c>
-      <c r="D61" t="s">
-        <v>172</v>
-      </c>
       <c r="F61" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I61" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2920,22 +2929,22 @@
         <v>2011</v>
       </c>
       <c r="C62" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D62" t="s">
         <v>9</v>
       </c>
       <c r="F62" t="s">
+        <v>117</v>
+      </c>
+      <c r="G62" t="s">
+        <v>119</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I62" t="s">
         <v>118</v>
-      </c>
-      <c r="G62" t="s">
-        <v>120</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="I62" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2946,22 +2955,22 @@
         <v>2011</v>
       </c>
       <c r="C63" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D63" t="s">
         <v>9</v>
       </c>
       <c r="F63" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G63" t="s">
+        <v>120</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I63" t="s">
         <v>121</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="I63" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
@@ -2972,19 +2981,19 @@
         <v>2011</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F64" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H64" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I64" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3001,13 +3010,13 @@
         <v>9</v>
       </c>
       <c r="F65" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I65" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -3030,7 +3039,7 @@
         <v>28</v>
       </c>
       <c r="H66" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I66" t="s">
         <v>32</v>
@@ -3050,7 +3059,7 @@
         <v>9</v>
       </c>
       <c r="G67" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3067,7 +3076,7 @@
         <v>15</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H68" s="1"/>
     </row>
@@ -3079,13 +3088,13 @@
         <v>2012</v>
       </c>
       <c r="C69" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D69" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H69" s="1"/>
     </row>
@@ -3103,7 +3112,7 @@
         <v>15</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H70" s="1"/>
     </row>
@@ -3121,7 +3130,7 @@
         <v>9</v>
       </c>
       <c r="G71" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
@@ -3138,7 +3147,7 @@
         <v>9</v>
       </c>
       <c r="G72" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3157,7 +3166,7 @@
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
       <c r="G73" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H73" s="5"/>
       <c r="I73" s="4"/>
@@ -3176,7 +3185,7 @@
         <v>15</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H74" s="1"/>
     </row>
@@ -3194,7 +3203,7 @@
         <v>9</v>
       </c>
       <c r="G75" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3205,13 +3214,13 @@
         <v>2013</v>
       </c>
       <c r="C76" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D76" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H76" s="1"/>
     </row>
@@ -3223,22 +3232,22 @@
         <v>2011</v>
       </c>
       <c r="C77" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D77" t="s">
         <v>9</v>
       </c>
       <c r="F77" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G77" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I77" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3249,19 +3258,19 @@
         <v>2011</v>
       </c>
       <c r="C78" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D78" t="s">
         <v>9</v>
       </c>
       <c r="G78" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I78" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3272,16 +3281,16 @@
         <v>2011</v>
       </c>
       <c r="C79" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D79" t="s">
         <v>15</v>
       </c>
       <c r="F79" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
@@ -3299,14 +3308,14 @@
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G80" s="4"/>
       <c r="H80" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
@@ -3328,7 +3337,7 @@
       </c>
       <c r="G81" s="4"/>
       <c r="H81" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I81" s="4" t="s">
         <v>39</v>
@@ -3349,14 +3358,14 @@
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G82" s="5"/>
       <c r="H82" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I82" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3374,14 +3383,14 @@
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G83" s="5"/>
       <c r="H83" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I83" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3392,15 +3401,15 @@
         <v>2014</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
       <c r="G84" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H84" s="5"/>
       <c r="I84" s="4"/>
@@ -3413,21 +3422,21 @@
         <v>2014</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G85" s="4"/>
       <c r="H85" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
@@ -3451,7 +3460,7 @@
         <v>29</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I86" s="4" t="s">
         <v>33</v>
@@ -3465,21 +3474,21 @@
         <v>2014</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G87" s="5"/>
       <c r="H87" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3490,21 +3499,21 @@
         <v>2014</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G88" s="5"/>
       <c r="H88" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3522,14 +3531,14 @@
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G89" s="5"/>
       <c r="H89" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
@@ -3549,7 +3558,7 @@
         <v>37</v>
       </c>
       <c r="H90" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I90" t="s">
         <v>50</v>
@@ -3572,13 +3581,13 @@
         <v>37</v>
       </c>
       <c r="G91" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H91" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I91" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
@@ -3598,7 +3607,7 @@
         <v>37</v>
       </c>
       <c r="H92" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I92" t="s">
         <v>38</v>
@@ -3622,7 +3631,7 @@
       </c>
       <c r="G93" s="1"/>
       <c r="H93" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I93" t="s">
         <v>48</v>
@@ -3642,7 +3651,7 @@
         <v>15</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H94" s="1"/>
       <c r="I94" s="3"/>
@@ -3655,17 +3664,17 @@
         <v>2015</v>
       </c>
       <c r="C95" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D95" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G95" s="1"/>
       <c r="H95" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I95" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
@@ -3682,13 +3691,13 @@
         <v>9</v>
       </c>
       <c r="F96" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H96" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I96" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
@@ -3708,7 +3717,7 @@
         <v>43</v>
       </c>
       <c r="H97" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I97" t="s">
         <v>14</v>
@@ -3722,20 +3731,20 @@
         <v>2016</v>
       </c>
       <c r="C98" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D98" t="s">
         <v>15</v>
       </c>
       <c r="F98" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G98" s="1"/>
       <c r="H98" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I98" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3752,11 +3761,11 @@
         <v>15</v>
       </c>
       <c r="F99" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G99" s="1"/>
       <c r="H99" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I99" t="s">
         <v>16</v>
@@ -3770,17 +3779,17 @@
         <v>2016</v>
       </c>
       <c r="C100" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D100" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G100" s="1"/>
       <c r="H100" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I100" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3800,10 +3809,10 @@
         <v>13</v>
       </c>
       <c r="H101" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I101" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3823,7 +3832,7 @@
         <v>13</v>
       </c>
       <c r="H102" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I102" t="s">
         <v>12</v>
@@ -3843,7 +3852,7 @@
         <v>15</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H103" s="1"/>
     </row>
@@ -3865,7 +3874,7 @@
       </c>
       <c r="G104" s="1"/>
       <c r="H104" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I104" t="s">
         <v>46</v>
@@ -3879,20 +3888,20 @@
         <v>2017</v>
       </c>
       <c r="C105" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D105" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F105" t="s">
         <v>13</v>
       </c>
       <c r="G105" s="1"/>
       <c r="H105" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I105" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
@@ -3903,19 +3912,19 @@
         <v>2017</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F106" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H106" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I106" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
@@ -3935,10 +3944,10 @@
         <v>26</v>
       </c>
       <c r="H107" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I107" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
@@ -3961,7 +3970,7 @@
         <v>30</v>
       </c>
       <c r="H108" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I108" t="s">
         <v>34</v>
@@ -3975,20 +3984,20 @@
         <v>2017</v>
       </c>
       <c r="C109" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D109" t="s">
         <v>15</v>
       </c>
       <c r="F109" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G109" s="1"/>
       <c r="H109" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4008,10 +4017,10 @@
         <v>76</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I110" t="s">
         <v>75</v>
@@ -4025,20 +4034,20 @@
         <v>2017</v>
       </c>
       <c r="C111" t="s">
+        <v>170</v>
+      </c>
+      <c r="D111" t="s">
         <v>171</v>
       </c>
-      <c r="D111" t="s">
-        <v>172</v>
-      </c>
       <c r="F111" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G111" s="1"/>
       <c r="H111" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I111" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4055,13 +4064,13 @@
         <v>9</v>
       </c>
       <c r="F112" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I112" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4081,10 +4090,10 @@
         <v>76</v>
       </c>
       <c r="G113" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I113" t="s">
         <v>74</v>
@@ -4104,13 +4113,13 @@
         <v>9</v>
       </c>
       <c r="F114" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H114" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I114" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4127,10 +4136,10 @@
         <v>9</v>
       </c>
       <c r="F115" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H115" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I115" t="s">
         <v>11</v>
@@ -4144,17 +4153,17 @@
         <v>2018</v>
       </c>
       <c r="C116" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D116" t="s">
         <v>15</v>
       </c>
       <c r="G116" s="1"/>
       <c r="H116" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I116" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4175,7 +4184,7 @@
       </c>
       <c r="G117" s="1"/>
       <c r="H117" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I117" t="s">
         <v>45</v>
@@ -4189,20 +4198,20 @@
         <v>2018</v>
       </c>
       <c r="C118" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D118" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F118" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G118" s="1"/>
       <c r="H118" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I118" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4213,20 +4222,20 @@
         <v>2018</v>
       </c>
       <c r="C119" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D119" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F119" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G119" s="1"/>
       <c r="H119" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I119" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4243,13 +4252,13 @@
         <v>9</v>
       </c>
       <c r="F120" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H120" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I120" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4269,7 +4278,7 @@
         <v>41</v>
       </c>
       <c r="H121" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I121" t="s">
         <v>10</v>
@@ -4283,17 +4292,17 @@
         <v>2019</v>
       </c>
       <c r="C122" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D122" t="s">
         <v>15</v>
       </c>
       <c r="G122" s="1"/>
       <c r="H122" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I122" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4304,20 +4313,20 @@
         <v>2019</v>
       </c>
       <c r="C123" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D123" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F123" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G123" s="1"/>
       <c r="H123" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I123" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="124" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4334,14 +4343,14 @@
         <v>15</v>
       </c>
       <c r="F124" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G124" s="1"/>
       <c r="H124" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I124" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4358,13 +4367,13 @@
         <v>9</v>
       </c>
       <c r="F125" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H125" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I125" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4384,7 +4393,7 @@
         <v>36</v>
       </c>
       <c r="H126" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I126" s="3" t="s">
         <v>8</v>
@@ -4398,13 +4407,13 @@
         <v>2020</v>
       </c>
       <c r="C127" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D127" t="s">
         <v>15</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H127" s="8"/>
     </row>
@@ -4426,7 +4435,7 @@
       </c>
       <c r="G128" s="1"/>
       <c r="H128" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I128" t="s">
         <v>35</v>
@@ -4440,20 +4449,20 @@
         <v>2020</v>
       </c>
       <c r="C129" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D129" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F129" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G129" s="1"/>
       <c r="H129" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I129" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4464,20 +4473,20 @@
         <v>2020</v>
       </c>
       <c r="C130" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D130" t="s">
         <v>15</v>
       </c>
       <c r="F130" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G130" s="1"/>
       <c r="H130" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I130" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4498,7 +4507,7 @@
       </c>
       <c r="G131" s="1"/>
       <c r="H131" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I131" t="s">
         <v>78</v>
@@ -4512,17 +4521,17 @@
         <v>2020</v>
       </c>
       <c r="C132" t="s">
+        <v>170</v>
+      </c>
+      <c r="D132" t="s">
         <v>171</v>
-      </c>
-      <c r="D132" t="s">
-        <v>172</v>
       </c>
       <c r="G132" s="1"/>
       <c r="H132" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I132" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4539,13 +4548,13 @@
         <v>9</v>
       </c>
       <c r="F133" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I133" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4556,19 +4565,19 @@
         <v>2020</v>
       </c>
       <c r="C134" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D134" t="s">
         <v>9</v>
       </c>
       <c r="F134" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H134" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I134" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4579,19 +4588,19 @@
         <v>2020</v>
       </c>
       <c r="C135" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D135" t="s">
         <v>15</v>
       </c>
       <c r="F135" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I135" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4611,7 +4620,7 @@
         <v>77</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I136" t="s">
         <v>73</v>
@@ -4634,10 +4643,10 @@
         <v>80</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I137" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4659,10 +4668,10 @@
       </c>
       <c r="G138" s="4"/>
       <c r="H138" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I138" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4673,17 +4682,17 @@
         <v>2021</v>
       </c>
       <c r="C139" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D139" t="s">
         <v>15</v>
       </c>
       <c r="G139" s="1"/>
       <c r="H139" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I139" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4704,7 +4713,7 @@
       </c>
       <c r="G140" s="1"/>
       <c r="H140" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I140" t="s">
         <v>79</v>
@@ -4718,20 +4727,20 @@
         <v>2021</v>
       </c>
       <c r="C141" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D141" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F141" t="s">
         <v>80</v>
       </c>
       <c r="G141" s="1"/>
       <c r="H141" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I141" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4751,10 +4760,10 @@
         <v>82</v>
       </c>
       <c r="H142" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I142" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4776,7 +4785,7 @@
       </c>
       <c r="G143" s="4"/>
       <c r="H143" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I143" s="4" t="s">
         <v>81</v>
@@ -4790,17 +4799,17 @@
         <v>2022</v>
       </c>
       <c r="C144" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D144" t="s">
         <v>15</v>
       </c>
       <c r="G144" s="1"/>
       <c r="H144" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I144" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4818,14 +4827,14 @@
       </c>
       <c r="E145" s="4"/>
       <c r="F145" s="4" t="s">
-        <v>82</v>
+        <v>319</v>
       </c>
       <c r="G145" s="5"/>
       <c r="H145" s="5" t="s">
-        <v>217</v>
+        <v>318</v>
       </c>
       <c r="I145" s="4" t="s">
-        <v>83</v>
+        <v>321</v>
       </c>
     </row>
     <row r="146" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4836,20 +4845,20 @@
         <v>2022</v>
       </c>
       <c r="C146" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D146" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F146" t="s">
         <v>82</v>
       </c>
       <c r="G146" s="1"/>
       <c r="H146" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I146" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4860,20 +4869,20 @@
         <v>2022</v>
       </c>
       <c r="C147" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D147" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F147" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G147" s="1"/>
       <c r="H147" s="10" t="s">
-        <v>217</v>
+        <v>318</v>
       </c>
       <c r="I147" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4890,66 +4899,66 @@
         <v>9</v>
       </c>
       <c r="F148" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="G148" s="1"/>
       <c r="H148" s="10" t="s">
-        <v>217</v>
+        <v>318</v>
       </c>
       <c r="I148" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="149" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>72</v>
+        <v>6</v>
       </c>
       <c r="B149">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="C149" t="s">
-        <v>238</v>
+        <v>49</v>
       </c>
       <c r="D149" t="s">
         <v>9</v>
       </c>
       <c r="F149" t="s">
-        <v>110</v>
-      </c>
-      <c r="G149" t="s">
-        <v>120</v>
-      </c>
-      <c r="H149" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="I149" s="3" t="s">
-        <v>246</v>
+        <v>319</v>
+      </c>
+      <c r="G149" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H149" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="I149" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="150" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>72</v>
+        <v>6</v>
       </c>
       <c r="B150">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="C150" t="s">
-        <v>238</v>
+        <v>49</v>
       </c>
       <c r="D150" t="s">
         <v>9</v>
       </c>
       <c r="F150" t="s">
-        <v>110</v>
-      </c>
-      <c r="G150" t="s">
-        <v>121</v>
-      </c>
-      <c r="H150" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="I150" s="3" t="s">
-        <v>245</v>
+        <v>319</v>
+      </c>
+      <c r="G150" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H150" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="I150" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4960,69 +4969,71 @@
         <v>2017</v>
       </c>
       <c r="C151" t="s">
-        <v>47</v>
+        <v>237</v>
       </c>
       <c r="D151" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F151" t="s">
-        <v>110</v>
+        <v>109</v>
+      </c>
+      <c r="G151" t="s">
+        <v>119</v>
       </c>
       <c r="H151" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="I151" t="s">
-        <v>242</v>
+        <v>220</v>
+      </c>
+      <c r="I151" s="3" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A152" s="4" t="s">
+      <c r="A152" t="s">
         <v>72</v>
       </c>
-      <c r="B152" s="4">
-        <v>2014</v>
-      </c>
-      <c r="C152" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D152" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E152" s="4"/>
-      <c r="F152" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="G152" s="5"/>
+      <c r="B152">
+        <v>2017</v>
+      </c>
+      <c r="C152" t="s">
+        <v>237</v>
+      </c>
+      <c r="D152" t="s">
+        <v>9</v>
+      </c>
+      <c r="F152" t="s">
+        <v>109</v>
+      </c>
+      <c r="G152" t="s">
+        <v>120</v>
+      </c>
       <c r="H152" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I152" s="4" t="s">
-        <v>174</v>
+      <c r="I152" s="3" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="153" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A153" s="4" t="s">
+      <c r="A153" t="s">
         <v>72</v>
       </c>
-      <c r="B153" s="4">
-        <v>2014</v>
-      </c>
-      <c r="C153" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D153" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E153" s="4"/>
-      <c r="F153" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G153" s="4"/>
+      <c r="B153">
+        <v>2017</v>
+      </c>
+      <c r="C153" t="s">
+        <v>47</v>
+      </c>
+      <c r="D153" t="s">
+        <v>15</v>
+      </c>
+      <c r="F153" t="s">
+        <v>109</v>
+      </c>
       <c r="H153" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I153" s="4" t="s">
-        <v>104</v>
+      <c r="I153" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5033,21 +5044,21 @@
         <v>2014</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>47</v>
+        <v>170</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>9</v>
+        <v>171</v>
       </c>
       <c r="E154" s="4"/>
       <c r="F154" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G154" s="4"/>
+        <v>175</v>
+      </c>
+      <c r="G154" s="5"/>
       <c r="H154" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I154" s="4" t="s">
-        <v>85</v>
+        <v>173</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5058,21 +5069,21 @@
         <v>2014</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>238</v>
+        <v>49</v>
       </c>
       <c r="D155" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E155" s="4"/>
       <c r="F155" s="4" t="s">
-        <v>247</v>
+        <v>104</v>
       </c>
       <c r="G155" s="4"/>
       <c r="H155" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="I155" s="11" t="s">
-        <v>241</v>
+        <v>219</v>
+      </c>
+      <c r="I155" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="156" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5083,67 +5094,71 @@
         <v>2014</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>238</v>
+        <v>47</v>
       </c>
       <c r="D156" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E156" s="4"/>
       <c r="F156" s="4" t="s">
-        <v>247</v>
+        <v>85</v>
       </c>
       <c r="G156" s="4"/>
       <c r="H156" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="I156" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="I156" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A157" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B157" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D157" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E157" s="4"/>
+      <c r="F157" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G157" s="4"/>
+      <c r="H157" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="I157" s="11" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="157" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
+    <row r="158" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A158" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B157">
-        <v>2008</v>
-      </c>
-      <c r="C157" t="s">
-        <v>238</v>
-      </c>
-      <c r="D157" t="s">
-        <v>9</v>
-      </c>
-      <c r="F157" t="s">
-        <v>60</v>
-      </c>
-      <c r="H157" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="I157" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="158" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
-        <v>72</v>
-      </c>
-      <c r="B158">
-        <v>2008</v>
-      </c>
-      <c r="C158" t="s">
-        <v>238</v>
-      </c>
-      <c r="D158" t="s">
+      <c r="B158" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C158" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D158" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F158" t="s">
-        <v>60</v>
-      </c>
+      <c r="E158" s="4"/>
+      <c r="F158" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G158" s="4"/>
       <c r="H158" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="I158" t="s">
-        <v>244</v>
+        <v>219</v>
+      </c>
+      <c r="I158" s="11" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5151,156 +5166,152 @@
         <v>72</v>
       </c>
       <c r="B159">
+        <v>2008</v>
+      </c>
+      <c r="C159" t="s">
+        <v>237</v>
+      </c>
+      <c r="D159" t="s">
+        <v>9</v>
+      </c>
+      <c r="F159" t="s">
+        <v>60</v>
+      </c>
+      <c r="H159" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="I159" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>72</v>
+      </c>
+      <c r="B160">
+        <v>2008</v>
+      </c>
+      <c r="C160" t="s">
+        <v>237</v>
+      </c>
+      <c r="D160" t="s">
+        <v>15</v>
+      </c>
+      <c r="F160" t="s">
+        <v>60</v>
+      </c>
+      <c r="H160" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="I160" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>72</v>
+      </c>
+      <c r="B161">
         <v>2017</v>
       </c>
-      <c r="C159" t="s">
-        <v>47</v>
-      </c>
-      <c r="D159" t="s">
-        <v>9</v>
-      </c>
-      <c r="F159" t="s">
-        <v>110</v>
-      </c>
-      <c r="G159" t="s">
-        <v>254</v>
-      </c>
-      <c r="H159" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="I159" t="s">
+      <c r="C161" t="s">
+        <v>47</v>
+      </c>
+      <c r="D161" t="s">
+        <v>9</v>
+      </c>
+      <c r="F161" t="s">
+        <v>109</v>
+      </c>
+      <c r="G161" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A160" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B160" s="4">
-        <v>2014</v>
-      </c>
-      <c r="C160" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="D160" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E160" s="4"/>
-      <c r="F160" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G160" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="H160" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="I160" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A161" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B161" s="4">
-        <v>2014</v>
-      </c>
-      <c r="C161" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="D161" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E161" s="4"/>
-      <c r="F161" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G161" s="4" t="s">
-        <v>121</v>
       </c>
       <c r="H161" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I161" s="11" t="s">
-        <v>258</v>
+      <c r="I161" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
-        <v>72</v>
+        <v>6</v>
       </c>
       <c r="B162" s="4">
         <v>2014</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D162" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E162" s="4"/>
       <c r="F162" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G162" s="4" t="s">
-        <v>260</v>
+        <v>119</v>
       </c>
       <c r="H162" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I162" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B163" s="4">
-        <v>2002</v>
+        <v>2014</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D163" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E163" s="4"/>
       <c r="F163" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="G163" s="4"/>
+        <v>93</v>
+      </c>
+      <c r="G163" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="H163" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="I163" s="4" t="s">
-        <v>261</v>
+        <v>219</v>
+      </c>
+      <c r="I163" s="11" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="B164" s="4">
-        <v>2005</v>
+        <v>2014</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D164" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E164" s="4"/>
       <c r="F164" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="G164" s="4"/>
+        <v>93</v>
+      </c>
+      <c r="G164" s="4" t="s">
+        <v>259</v>
+      </c>
       <c r="H164" s="5" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
       <c r="I164" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5308,24 +5319,24 @@
         <v>5</v>
       </c>
       <c r="B165" s="4">
-        <v>2008</v>
+        <v>2002</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D165" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E165" s="4"/>
       <c r="F165" s="4" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G165" s="4"/>
       <c r="H165" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I165" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5333,24 +5344,24 @@
         <v>5</v>
       </c>
       <c r="B166" s="4">
-        <v>2011</v>
+        <v>2005</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D166" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E166" s="4"/>
       <c r="F166" s="4" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G166" s="4"/>
       <c r="H166" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I166" s="4" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="167" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5358,24 +5369,24 @@
         <v>5</v>
       </c>
       <c r="B167" s="4">
-        <v>2014</v>
+        <v>2008</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D167" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E167" s="4"/>
       <c r="F167" s="4" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G167" s="4"/>
       <c r="H167" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I167" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="168" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5383,24 +5394,24 @@
         <v>5</v>
       </c>
       <c r="B168" s="4">
-        <v>2017</v>
+        <v>2011</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D168" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E168" s="4"/>
       <c r="F168" s="4" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G168" s="4"/>
       <c r="H168" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I168" s="4" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5408,26 +5419,24 @@
         <v>5</v>
       </c>
       <c r="B169" s="4">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D169" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E169" s="4"/>
       <c r="F169" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="G169" s="4" t="s">
-        <v>269</v>
-      </c>
+        <v>312</v>
+      </c>
+      <c r="G169" s="4"/>
       <c r="H169" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I169" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="170" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5435,26 +5444,24 @@
         <v>5</v>
       </c>
       <c r="B170" s="4">
-        <v>2002</v>
+        <v>2017</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D170" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E170" s="4"/>
-      <c r="F170" t="s">
-        <v>308</v>
-      </c>
-      <c r="G170" s="4" t="s">
-        <v>291</v>
-      </c>
+      <c r="F170" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="G170" s="4"/>
       <c r="H170" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I170" s="4" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5462,26 +5469,26 @@
         <v>5</v>
       </c>
       <c r="B171" s="4">
-        <v>2003</v>
+        <v>2019</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D171" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E171" s="4"/>
-      <c r="F171" t="s">
-        <v>292</v>
+      <c r="F171" s="4" t="s">
+        <v>314</v>
       </c>
       <c r="G171" s="4" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
       <c r="H171" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I171" s="4" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="172" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5489,26 +5496,26 @@
         <v>5</v>
       </c>
       <c r="B172" s="4">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D172" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E172" s="4"/>
       <c r="F172" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="G172" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H172" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I172" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5516,26 +5523,26 @@
         <v>5</v>
       </c>
       <c r="B173" s="4">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D173" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E173" s="4"/>
       <c r="F173" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G173" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H173" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I173" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="174" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5543,26 +5550,26 @@
         <v>5</v>
       </c>
       <c r="B174" s="4">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D174" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E174" s="4"/>
       <c r="F174" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="G174" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H174" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I174" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="175" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5570,26 +5577,26 @@
         <v>5</v>
       </c>
       <c r="B175" s="4">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D175" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E175" s="4"/>
       <c r="F175" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="G175" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H175" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I175" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="176" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5597,26 +5604,26 @@
         <v>5</v>
       </c>
       <c r="B176" s="4">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D176" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E176" s="4"/>
       <c r="F176" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G176" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H176" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I176" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="177" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5624,26 +5631,26 @@
         <v>5</v>
       </c>
       <c r="B177" s="4">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D177" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E177" s="4"/>
       <c r="F177" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G177" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H177" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="I177" s="11" t="s">
-        <v>280</v>
+        <v>267</v>
+      </c>
+      <c r="I177" s="4" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="178" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5651,26 +5658,26 @@
         <v>5</v>
       </c>
       <c r="B178" s="4">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D178" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E178" s="4"/>
       <c r="F178" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G178" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H178" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I178" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="179" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5678,26 +5685,26 @@
         <v>5</v>
       </c>
       <c r="B179" s="4">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D179" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E179" s="4"/>
       <c r="F179" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G179" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H179" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="I179" s="4" t="s">
-        <v>282</v>
+        <v>267</v>
+      </c>
+      <c r="I179" s="11" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="180" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5705,26 +5712,26 @@
         <v>5</v>
       </c>
       <c r="B180" s="4">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D180" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E180" s="4"/>
       <c r="F180" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G180" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H180" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I180" s="4" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="181" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5732,26 +5739,26 @@
         <v>5</v>
       </c>
       <c r="B181" s="4">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D181" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E181" s="4"/>
       <c r="F181" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G181" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H181" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I181" s="4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5759,26 +5766,26 @@
         <v>5</v>
       </c>
       <c r="B182" s="4">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D182" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E182" s="4"/>
       <c r="F182" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G182" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H182" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I182" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="183" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5786,26 +5793,26 @@
         <v>5</v>
       </c>
       <c r="B183" s="4">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D183" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E183" s="4"/>
       <c r="F183" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G183" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H183" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I183" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="184" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5813,26 +5820,26 @@
         <v>5</v>
       </c>
       <c r="B184" s="4">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D184" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E184" s="4"/>
       <c r="F184" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G184" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H184" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I184" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5840,26 +5847,26 @@
         <v>5</v>
       </c>
       <c r="B185" s="4">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D185" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E185" s="4"/>
       <c r="F185" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="G185" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H185" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I185" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="186" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5867,26 +5874,26 @@
         <v>5</v>
       </c>
       <c r="B186" s="4">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D186" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E186" s="4"/>
       <c r="F186" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G186" s="4" t="s">
-        <v>316</v>
+        <v>290</v>
       </c>
       <c r="H186" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I186" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="187" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -5894,32 +5901,86 @@
         <v>5</v>
       </c>
       <c r="B187" s="4">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D187" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E187" s="4"/>
       <c r="F187" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G187" s="4" t="s">
-        <v>316</v>
+        <v>290</v>
       </c>
       <c r="H187" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I187" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A188" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B188" s="4">
+        <v>2018</v>
+      </c>
+      <c r="C188" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D188" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E188" s="4"/>
+      <c r="F188" t="s">
+        <v>305</v>
+      </c>
+      <c r="G188" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="H188" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="I188" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A189" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B189" s="4">
+        <v>2019</v>
+      </c>
+      <c r="C189" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D189" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E189" s="4"/>
+      <c r="F189" t="s">
+        <v>306</v>
+      </c>
+      <c r="G189" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="H189" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="I189" s="4" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I187" xr:uid="{EB8EF959-18DF-BD43-B878-2D065289D72D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A53:I156">
-      <sortCondition ref="B1:B158"/>
+  <autoFilter ref="A1:I189" xr:uid="{EB8EF959-18DF-BD43-B878-2D065289D72D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A53:I158">
+      <sortCondition ref="B1:B160"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:I146">
@@ -5957,10 +6018,10 @@
     <hyperlink ref="I24" r:id="rId9" xr:uid="{9F3A0EC8-88EF-BA42-B2C4-CD63FAF3743E}"/>
     <hyperlink ref="I83" r:id="rId10" xr:uid="{89E45E83-4EF9-8B44-AACC-ED2D2E60F75C}"/>
     <hyperlink ref="I135" r:id="rId11" xr:uid="{FA8A1007-708D-DF45-A09D-78C317607EA1}"/>
-    <hyperlink ref="I155" r:id="rId12" xr:uid="{8AB8E0D9-B2E6-7A4B-B7FD-383AE4C17BF2}"/>
-    <hyperlink ref="I156" r:id="rId13" xr:uid="{6702C906-A8EA-954F-8C17-7147195B6C53}"/>
-    <hyperlink ref="I161" r:id="rId14" xr:uid="{AFDA6783-AFA0-A040-820E-4E25136EB298}"/>
-    <hyperlink ref="I177" r:id="rId15" xr:uid="{DD2C4424-579F-DF41-A73A-7ECFAD2F604F}"/>
+    <hyperlink ref="I157" r:id="rId12" xr:uid="{8AB8E0D9-B2E6-7A4B-B7FD-383AE4C17BF2}"/>
+    <hyperlink ref="I158" r:id="rId13" xr:uid="{6702C906-A8EA-954F-8C17-7147195B6C53}"/>
+    <hyperlink ref="I163" r:id="rId14" xr:uid="{AFDA6783-AFA0-A040-820E-4E25136EB298}"/>
+    <hyperlink ref="I179" r:id="rId15" xr:uid="{DD2C4424-579F-DF41-A73A-7ECFAD2F604F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5985,7 +6046,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -5993,7 +6054,7 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -6001,7 +6062,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -6009,15 +6070,15 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B5" t="s">
         <v>270</v>
-      </c>
-      <c r="B5" t="s">
-        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -6037,37 +6098,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>